<commit_message>
Fixed FMWT and STN data issues
</commit_message>
<xml_diff>
--- a/data-raw/stations.xlsx
+++ b/data-raw/stations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D437EDA0-0B3D-44DB-BA5B-6D5EBABFBF1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723A3C4-9E23-4F45-B0DC-60C60C0294D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1125" windowWidth="18285" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lat_long" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="453">
   <si>
     <t>Project</t>
   </si>
@@ -1383,6 +1383,15 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>Mont</t>
+  </si>
+  <si>
+    <t>Honk</t>
+  </si>
+  <si>
+    <t>FRP Grizz</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1403,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1439,6 +1448,24 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1617,14 +1644,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1723,9 +1751,19 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{20E71925-2C43-42B8-A035-0F7930C15447}"/>
     <cellStyle name="Normal_Sheet3" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal_Station Import" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal_Station Lookup" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -2007,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G431"/>
+  <dimension ref="A1:G434"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4375,26 +4413,44 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="B172" s="33">
-        <v>997</v>
+        <v>238</v>
+      </c>
+      <c r="B172" s="48" t="s">
+        <v>450</v>
+      </c>
+      <c r="C172" s="49">
+        <v>38.143865830000003</v>
+      </c>
+      <c r="D172" s="49">
+        <v>-121.90888889</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="B173" s="33">
-        <v>998</v>
+        <v>238</v>
+      </c>
+      <c r="B173" s="48" t="s">
+        <v>451</v>
+      </c>
+      <c r="C173" s="49">
+        <v>38.072800000000001</v>
+      </c>
+      <c r="D173" s="49">
+        <v>-121.92111111</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="B174" s="33">
-        <v>999</v>
+        <v>238</v>
+      </c>
+      <c r="B174" s="48" t="s">
+        <v>452</v>
+      </c>
+      <c r="C174" s="50">
+        <v>38.113421000000002</v>
+      </c>
+      <c r="D174" s="49">
+        <v>-121.98896999999999</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4402,13 +4458,7 @@
         <v>448</v>
       </c>
       <c r="B175" s="33">
-        <v>323</v>
-      </c>
-      <c r="C175" s="29">
-        <v>38.042888888888889</v>
-      </c>
-      <c r="D175" s="29">
-        <v>-122.28630555555556</v>
+        <v>997</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4416,13 +4466,7 @@
         <v>448</v>
       </c>
       <c r="B176" s="33">
-        <v>328</v>
-      </c>
-      <c r="C176" s="29">
-        <v>38.060305555555551</v>
-      </c>
-      <c r="D176" s="29">
-        <v>-122.35</v>
+        <v>998</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4430,13 +4474,7 @@
         <v>448</v>
       </c>
       <c r="B177" s="33">
-        <v>329</v>
-      </c>
-      <c r="C177" s="29">
-        <v>38.063611111111108</v>
-      </c>
-      <c r="D177" s="29">
-        <v>-122.304</v>
+        <v>999</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4444,13 +4482,13 @@
         <v>448</v>
       </c>
       <c r="B178" s="33">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C178" s="29">
-        <v>38.076388888888893</v>
+        <v>38.042888888888889</v>
       </c>
       <c r="D178" s="29">
-        <v>-122.33799999999999</v>
+        <v>-122.28630555555556</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4458,13 +4496,13 @@
         <v>448</v>
       </c>
       <c r="B179" s="33">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C179" s="29">
-        <v>38.071111111111115</v>
+        <v>38.060305555555551</v>
       </c>
       <c r="D179" s="29">
-        <v>-122.324</v>
+        <v>-122.35</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4472,13 +4510,13 @@
         <v>448</v>
       </c>
       <c r="B180" s="33">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C180" s="29">
-        <v>38.061083333333329</v>
+        <v>38.063611111111108</v>
       </c>
       <c r="D180" s="29">
-        <v>-122.27800000000001</v>
+        <v>-122.304</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4486,13 +4524,13 @@
         <v>448</v>
       </c>
       <c r="B181" s="33">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C181" s="29">
-        <v>38.099222222222224</v>
+        <v>38.076388888888893</v>
       </c>
       <c r="D181" s="29">
-        <v>-122.26327777777777</v>
+        <v>-122.33799999999999</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4500,13 +4538,13 @@
         <v>448</v>
       </c>
       <c r="B182" s="33">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C182" s="29">
-        <v>38.127250000000004</v>
+        <v>38.071111111111115</v>
       </c>
       <c r="D182" s="29">
-        <v>-122.27877777777778</v>
+        <v>-122.324</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4514,13 +4552,13 @@
         <v>448</v>
       </c>
       <c r="B183" s="33">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C183" s="29">
-        <v>38.146250000000002</v>
+        <v>38.061083333333329</v>
       </c>
       <c r="D183" s="29">
-        <v>-122.28874999999999</v>
+        <v>-122.27800000000001</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4528,13 +4566,13 @@
         <v>448</v>
       </c>
       <c r="B184" s="33">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C184" s="29">
-        <v>38.182361111111106</v>
+        <v>38.099222222222224</v>
       </c>
       <c r="D184" s="29">
-        <v>-122.30927777777778</v>
+        <v>-122.26327777777777</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4542,13 +4580,13 @@
         <v>448</v>
       </c>
       <c r="B185" s="33">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C185" s="29">
-        <v>38.212694444444445</v>
+        <v>38.127250000000004</v>
       </c>
       <c r="D185" s="29">
-        <v>-122.30869444444444</v>
+        <v>-122.27877777777778</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4556,13 +4594,13 @@
         <v>448</v>
       </c>
       <c r="B186" s="33">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C186" s="29">
-        <v>38.223833333333339</v>
+        <v>38.146250000000002</v>
       </c>
       <c r="D186" s="29">
-        <v>-122.30897222222222</v>
+        <v>-122.28874999999999</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4570,13 +4608,13 @@
         <v>448</v>
       </c>
       <c r="B187" s="33">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C187" s="29">
-        <v>38.236388888888889</v>
+        <v>38.182361111111106</v>
       </c>
       <c r="D187" s="29">
-        <v>-122.28716666666666</v>
+        <v>-122.30927777777778</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4584,13 +4622,13 @@
         <v>448</v>
       </c>
       <c r="B188" s="33">
-        <v>405</v>
+        <v>344</v>
       </c>
       <c r="C188" s="29">
-        <v>38.039916666666663</v>
+        <v>38.212694444444445</v>
       </c>
       <c r="D188" s="29">
-        <v>-122.14672222222222</v>
+        <v>-122.30869444444444</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4598,13 +4636,13 @@
         <v>448</v>
       </c>
       <c r="B189" s="33">
-        <v>411</v>
+        <v>345</v>
       </c>
       <c r="C189" s="29">
-        <v>38.050222222222217</v>
+        <v>38.223833333333339</v>
       </c>
       <c r="D189" s="29">
-        <v>-122.07652777777777</v>
+        <v>-122.30897222222222</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4612,13 +4650,13 @@
         <v>448</v>
       </c>
       <c r="B190" s="33">
-        <v>418</v>
+        <v>346</v>
       </c>
       <c r="C190" s="29">
-        <v>38.067500000000003</v>
+        <v>38.236388888888889</v>
       </c>
       <c r="D190" s="29">
-        <v>-122.09555555555555</v>
+        <v>-122.28716666666666</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4626,13 +4664,13 @@
         <v>448</v>
       </c>
       <c r="B191" s="33">
-        <v>501</v>
+        <v>405</v>
       </c>
       <c r="C191" s="29">
-        <v>38.073333333333338</v>
+        <v>38.039916666666663</v>
       </c>
       <c r="D191" s="29">
-        <v>-122.02633333333333</v>
+        <v>-122.14672222222222</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4640,13 +4678,13 @@
         <v>448</v>
       </c>
       <c r="B192" s="33">
-        <v>504</v>
+        <v>411</v>
       </c>
       <c r="C192" s="29">
-        <v>38.051944444444445</v>
+        <v>38.050222222222217</v>
       </c>
       <c r="D192" s="29">
-        <v>-121.98608333333334</v>
+        <v>-122.07652777777777</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4654,13 +4692,13 @@
         <v>448</v>
       </c>
       <c r="B193" s="33">
-        <v>508</v>
+        <v>418</v>
       </c>
       <c r="C193" s="29">
-        <v>38.047166666666662</v>
+        <v>38.067500000000003</v>
       </c>
       <c r="D193" s="29">
-        <v>-121.91722222222222</v>
+        <v>-122.09555555555555</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4668,13 +4706,13 @@
         <v>448</v>
       </c>
       <c r="B194" s="33">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="C194" s="29">
-        <v>38.058861111111106</v>
+        <v>38.073333333333338</v>
       </c>
       <c r="D194" s="29">
-        <v>-121.86774999999999</v>
+        <v>-122.02633333333333</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4682,13 +4720,13 @@
         <v>448</v>
       </c>
       <c r="B195" s="33">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="C195" s="29">
-        <v>38.074750000000002</v>
+        <v>38.051944444444445</v>
       </c>
       <c r="D195" s="29">
-        <v>-121.95808333333333</v>
+        <v>-121.98608333333334</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4696,13 +4734,13 @@
         <v>448</v>
       </c>
       <c r="B196" s="33">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="C196" s="29">
-        <v>38.032166666666669</v>
+        <v>38.047166666666662</v>
       </c>
       <c r="D196" s="29">
-        <v>-121.86311111111111</v>
+        <v>-121.91722222222222</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4710,13 +4748,13 @@
         <v>448</v>
       </c>
       <c r="B197" s="33">
-        <v>602</v>
+        <v>513</v>
       </c>
       <c r="C197" s="29">
-        <v>38.115555555555559</v>
+        <v>38.058861111111106</v>
       </c>
       <c r="D197" s="29">
-        <v>-122.04239166666666</v>
+        <v>-121.86774999999999</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4724,13 +4762,13 @@
         <v>448</v>
       </c>
       <c r="B198" s="33">
-        <v>606</v>
+        <v>519</v>
       </c>
       <c r="C198" s="29">
-        <v>38.170583333333333</v>
+        <v>38.074750000000002</v>
       </c>
       <c r="D198" s="29">
-        <v>-122.02791666666667</v>
+        <v>-121.95808333333333</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4738,13 +4776,13 @@
         <v>448</v>
       </c>
       <c r="B199" s="33">
-        <v>609</v>
+        <v>520</v>
       </c>
       <c r="C199" s="29">
-        <v>38.167083333333331</v>
+        <v>38.032166666666669</v>
       </c>
       <c r="D199" s="29">
-        <v>-121.93783333333333</v>
+        <v>-121.86311111111111</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4752,13 +4790,13 @@
         <v>448</v>
       </c>
       <c r="B200" s="33">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C200" s="29">
-        <v>38.122194444444446</v>
+        <v>38.115555555555559</v>
       </c>
       <c r="D200" s="29">
-        <v>-121.88911111111112</v>
+        <v>-122.04239166666666</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -4766,13 +4804,13 @@
         <v>448</v>
       </c>
       <c r="B201" s="33">
-        <v>703</v>
+        <v>606</v>
       </c>
       <c r="C201" s="29">
-        <v>38.048611111111107</v>
+        <v>38.170583333333333</v>
       </c>
       <c r="D201" s="29">
-        <v>-121.79738888888889</v>
+        <v>-122.02791666666667</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -4780,29 +4818,27 @@
         <v>448</v>
       </c>
       <c r="B202" s="33">
-        <v>704</v>
+        <v>609</v>
       </c>
       <c r="C202" s="29">
-        <v>38.066583333333334</v>
+        <v>38.167083333333331</v>
       </c>
       <c r="D202" s="29">
-        <v>-121.79031111111111</v>
-      </c>
-      <c r="F202" s="24"/>
-      <c r="G202" s="24"/>
+        <v>-121.93783333333333</v>
+      </c>
     </row>
     <row r="203" spans="1:7">
       <c r="A203" s="32" t="s">
         <v>448</v>
       </c>
       <c r="B203" s="33">
-        <v>705</v>
+        <v>610</v>
       </c>
       <c r="C203" s="29">
-        <v>38.097611111111114</v>
+        <v>38.122194444444446</v>
       </c>
       <c r="D203" s="29">
-        <v>-121.70875000000001</v>
+        <v>-121.88911111111112</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -4810,13 +4846,13 @@
         <v>448</v>
       </c>
       <c r="B204" s="33">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C204" s="29">
-        <v>38.086083333333335</v>
+        <v>38.048611111111107</v>
       </c>
       <c r="D204" s="29">
-        <v>-121.75044444444444</v>
+        <v>-121.79738888888889</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -4824,27 +4860,29 @@
         <v>448</v>
       </c>
       <c r="B205" s="33">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C205" s="29">
-        <v>38.114694444444446</v>
+        <v>38.066583333333334</v>
       </c>
       <c r="D205" s="29">
-        <v>-121.70786111111111</v>
-      </c>
+        <v>-121.79031111111111</v>
+      </c>
+      <c r="F205" s="24"/>
+      <c r="G205" s="24"/>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="32" t="s">
         <v>448</v>
       </c>
       <c r="B206" s="33">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="C206" s="29">
-        <v>38.177416666666666</v>
+        <v>38.097611111111114</v>
       </c>
       <c r="D206" s="29">
-        <v>-121.66225</v>
+        <v>-121.70875000000001</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -4852,13 +4890,13 @@
         <v>448</v>
       </c>
       <c r="B207" s="33">
-        <v>716</v>
+        <v>706</v>
       </c>
       <c r="C207" s="29">
-        <v>38.238555555555557</v>
+        <v>38.086083333333335</v>
       </c>
       <c r="D207" s="29">
-        <v>-121.68391666666668</v>
+        <v>-121.75044444444444</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -4866,13 +4904,13 @@
         <v>448</v>
       </c>
       <c r="B208" s="33">
-        <v>801</v>
+        <v>707</v>
       </c>
       <c r="C208" s="29">
-        <v>38.043694444444441</v>
+        <v>38.114694444444446</v>
       </c>
       <c r="D208" s="29">
-        <v>-121.84399999999999</v>
+        <v>-121.70786111111111</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4880,13 +4918,13 @@
         <v>448</v>
       </c>
       <c r="B209" s="33">
-        <v>802</v>
+        <v>711</v>
       </c>
       <c r="C209" s="29">
-        <v>38.020833333333336</v>
+        <v>38.177416666666666</v>
       </c>
       <c r="D209" s="29">
-        <v>-121.7303888888889</v>
+        <v>-121.66225</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4894,13 +4932,13 @@
         <v>448</v>
       </c>
       <c r="B210" s="33">
-        <v>804</v>
+        <v>716</v>
       </c>
       <c r="C210" s="29">
-        <v>38.016444444444446</v>
+        <v>38.238555555555557</v>
       </c>
       <c r="D210" s="29">
-        <v>-121.79130555555555</v>
+        <v>-121.68391666666668</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4908,13 +4946,13 @@
         <v>448</v>
       </c>
       <c r="B211" s="33">
-        <v>809</v>
+        <v>801</v>
       </c>
       <c r="C211" s="29">
-        <v>38.053777777777775</v>
+        <v>38.043694444444441</v>
       </c>
       <c r="D211" s="29">
-        <v>-121.69302777777779</v>
+        <v>-121.84399999999999</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4922,13 +4960,13 @@
         <v>448</v>
       </c>
       <c r="B212" s="33">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="C212" s="29">
-        <v>38.089916666666667</v>
+        <v>38.020833333333336</v>
       </c>
       <c r="D212" s="29">
-        <v>-121.63991666666668</v>
+        <v>-121.7303888888889</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4936,13 +4974,13 @@
         <v>448</v>
       </c>
       <c r="B213" s="33">
-        <v>815</v>
+        <v>804</v>
       </c>
       <c r="C213" s="29">
-        <v>38.087138888888894</v>
+        <v>38.016444444444446</v>
       </c>
       <c r="D213" s="29">
-        <v>-121.57113888888888</v>
+        <v>-121.79130555555555</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4950,13 +4988,13 @@
         <v>448</v>
       </c>
       <c r="B214" s="33">
-        <v>901</v>
+        <v>809</v>
       </c>
       <c r="C214" s="29">
-        <v>38.046250000000001</v>
+        <v>38.053777777777775</v>
       </c>
       <c r="D214" s="29">
-        <v>-121.6185</v>
+        <v>-121.69302777777779</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4964,13 +5002,13 @@
         <v>448</v>
       </c>
       <c r="B215" s="33">
-        <v>902</v>
+        <v>812</v>
       </c>
       <c r="C215" s="29">
-        <v>38.020388888888888</v>
+        <v>38.089916666666667</v>
       </c>
       <c r="D215" s="29">
-        <v>-121.58266666666667</v>
+        <v>-121.63991666666668</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4978,13 +5016,13 @@
         <v>448</v>
       </c>
       <c r="B216" s="33">
-        <v>906</v>
+        <v>815</v>
       </c>
       <c r="C216" s="29">
-        <v>38.050027777777778</v>
+        <v>38.087138888888894</v>
       </c>
       <c r="D216" s="29">
-        <v>-121.50647222222223</v>
+        <v>-121.57113888888888</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4992,13 +5030,13 @@
         <v>448</v>
       </c>
       <c r="B217" s="33">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="C217" s="29">
-        <v>38.005000000000003</v>
+        <v>38.046250000000001</v>
       </c>
       <c r="D217" s="29">
-        <v>-121.45302777777778</v>
+        <v>-121.6185</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -5006,13 +5044,13 @@
         <v>448</v>
       </c>
       <c r="B218" s="33">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="C218" s="29">
-        <v>37.966416666666667</v>
+        <v>38.020388888888888</v>
       </c>
       <c r="D218" s="29">
-        <v>-121.36855555555555</v>
+        <v>-121.58266666666667</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -5020,13 +5058,13 @@
         <v>448</v>
       </c>
       <c r="B219" s="33">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="C219" s="29">
-        <v>37.971499999999999</v>
+        <v>38.050027777777778</v>
       </c>
       <c r="D219" s="29">
-        <v>-121.52</v>
+        <v>-121.50647222222223</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -5034,13 +5072,13 @@
         <v>448</v>
       </c>
       <c r="B220" s="33">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="C220" s="29">
-        <v>37.944277777777778</v>
+        <v>38.005000000000003</v>
       </c>
       <c r="D220" s="29">
-        <v>-121.56788888888889</v>
+        <v>-121.45302777777778</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -5048,13 +5086,13 @@
         <v>448</v>
       </c>
       <c r="B221" s="33">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="C221" s="29">
-        <v>37.859000000000002</v>
+        <v>37.966416666666667</v>
       </c>
       <c r="D221" s="29">
-        <v>-121.56713888888889</v>
+        <v>-121.36855555555555</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5062,13 +5100,13 @@
         <v>448</v>
       </c>
       <c r="B222" s="33">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="C222" s="29">
-        <v>38.105194444444443</v>
+        <v>37.971499999999999</v>
       </c>
       <c r="D222" s="29">
-        <v>-121.49458333333334</v>
+        <v>-121.52</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5076,13 +5114,13 @@
         <v>448</v>
       </c>
       <c r="B223" s="33">
-        <v>330</v>
+        <v>915</v>
       </c>
       <c r="C223" s="29">
-        <v>38.063611111111108</v>
+        <v>37.944277777777778</v>
       </c>
       <c r="D223" s="29">
-        <v>-122.304</v>
+        <v>-121.56788888888889</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5090,13 +5128,13 @@
         <v>448</v>
       </c>
       <c r="B224" s="33">
-        <v>347</v>
+        <v>918</v>
       </c>
       <c r="C224" s="29">
-        <v>38.253611111111113</v>
+        <v>37.859000000000002</v>
       </c>
       <c r="D224" s="29">
-        <v>-122.28469444444444</v>
+        <v>-121.56713888888889</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5104,13 +5142,13 @@
         <v>448</v>
       </c>
       <c r="B225" s="33">
-        <v>348</v>
+        <v>919</v>
       </c>
       <c r="C225" s="29">
-        <v>38.274361111111112</v>
+        <v>38.105194444444443</v>
       </c>
       <c r="D225" s="29">
-        <v>-122.28352777777778</v>
+        <v>-121.49458333333334</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5118,13 +5156,13 @@
         <v>448</v>
       </c>
       <c r="B226" s="33">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="C226" s="29">
-        <v>38.286333333333332</v>
+        <v>38.063611111111108</v>
       </c>
       <c r="D226" s="29">
-        <v>-122.28436111111111</v>
+        <v>-122.304</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5132,13 +5170,13 @@
         <v>448</v>
       </c>
       <c r="B227" s="33">
-        <v>718</v>
+        <v>347</v>
       </c>
       <c r="C227" s="29">
-        <v>38.257555555555555</v>
+        <v>38.253611111111113</v>
       </c>
       <c r="D227" s="29">
-        <v>-121.72902777777777</v>
+        <v>-122.28469444444444</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5146,13 +5184,13 @@
         <v>448</v>
       </c>
       <c r="B228" s="33">
-        <v>720</v>
+        <v>348</v>
       </c>
       <c r="C228" s="29">
-        <v>38.262638888888887</v>
+        <v>38.274361111111112</v>
       </c>
       <c r="D228" s="29">
-        <v>-121.77927777777778</v>
+        <v>-122.28352777777778</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5160,13 +5198,13 @@
         <v>448</v>
       </c>
       <c r="B229" s="33">
-        <v>723</v>
+        <v>349</v>
       </c>
       <c r="C229" s="29">
-        <v>38.237250000000003</v>
+        <v>38.286333333333332</v>
       </c>
       <c r="D229" s="29">
-        <v>-121.67308333333334</v>
+        <v>-122.28436111111111</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5174,13 +5212,13 @@
         <v>448</v>
       </c>
       <c r="B230" s="33">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C230" s="29">
-        <v>38.256250000000001</v>
+        <v>38.257555555555555</v>
       </c>
       <c r="D230" s="29">
-        <v>-121.65208333333334</v>
+        <v>-121.72902777777777</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5188,7 +5226,13 @@
         <v>448</v>
       </c>
       <c r="B231" s="33">
-        <v>794</v>
+        <v>720</v>
+      </c>
+      <c r="C231" s="29">
+        <v>38.262638888888887</v>
+      </c>
+      <c r="D231" s="29">
+        <v>-121.77927777777778</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5196,7 +5240,13 @@
         <v>448</v>
       </c>
       <c r="B232" s="33">
-        <v>795</v>
+        <v>723</v>
+      </c>
+      <c r="C232" s="29">
+        <v>38.237250000000003</v>
+      </c>
+      <c r="D232" s="29">
+        <v>-121.67308333333334</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5204,7 +5254,13 @@
         <v>448</v>
       </c>
       <c r="B233" s="33">
-        <v>796</v>
+        <v>724</v>
+      </c>
+      <c r="C233" s="29">
+        <v>38.256250000000001</v>
+      </c>
+      <c r="D233" s="29">
+        <v>-121.65208333333334</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5212,7 +5268,7 @@
         <v>448</v>
       </c>
       <c r="B234" s="33">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5220,7 +5276,7 @@
         <v>448</v>
       </c>
       <c r="B235" s="33">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5228,7 +5284,7 @@
         <v>448</v>
       </c>
       <c r="B236" s="33">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5236,13 +5292,7 @@
         <v>448</v>
       </c>
       <c r="B237" s="33">
-        <v>726</v>
-      </c>
-      <c r="C237" s="29">
-        <v>38.283055555555556</v>
-      </c>
-      <c r="D237" s="29">
-        <v>-121.64383333333333</v>
+        <v>797</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5250,55 +5300,43 @@
         <v>448</v>
       </c>
       <c r="B238" s="33">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B239" s="33">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B240" s="33">
+        <v>726</v>
+      </c>
+      <c r="C240" s="29">
+        <v>38.283055555555556</v>
+      </c>
+      <c r="D240" s="29">
+        <v>-121.64383333333333</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B241" s="33">
         <v>719</v>
       </c>
-      <c r="C238" s="29">
+      <c r="C241" s="29">
         <v>38.333500000000001</v>
       </c>
-      <c r="D238" s="29">
+      <c r="D241" s="29">
         <v>-121.64750000000001</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4">
-      <c r="A239" s="28" t="s">
-        <v>391</v>
-      </c>
-      <c r="B239" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C239" s="30">
-        <v>38.074469999999998</v>
-      </c>
-      <c r="D239" s="30">
-        <v>-122.01588</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4">
-      <c r="A240" s="28" t="s">
-        <v>391</v>
-      </c>
-      <c r="B240" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="C240" s="30">
-        <v>38.044820000000001</v>
-      </c>
-      <c r="D240" s="30">
-        <v>-121.87193000000001</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4">
-      <c r="A241" s="28" t="s">
-        <v>391</v>
-      </c>
-      <c r="B241" s="30" t="s">
-        <v>253</v>
-      </c>
-      <c r="C241" s="30">
-        <v>38.121292169999997</v>
-      </c>
-      <c r="D241" s="30">
-        <v>-122.0067224</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5306,13 +5344,13 @@
         <v>391</v>
       </c>
       <c r="B242" s="30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C242" s="30">
-        <v>38.181780430000003</v>
+        <v>38.074469999999998</v>
       </c>
       <c r="D242" s="30">
-        <v>-121.91393739999999</v>
+        <v>-122.01588</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5320,13 +5358,13 @@
         <v>391</v>
       </c>
       <c r="B243" s="30" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C243" s="30">
-        <v>38.043095299999997</v>
+        <v>38.044820000000001</v>
       </c>
       <c r="D243" s="30">
-        <v>-121.7992028</v>
+        <v>-121.87193000000001</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5334,13 +5372,13 @@
         <v>391</v>
       </c>
       <c r="B244" s="30" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C244" s="30">
-        <v>38.08988506</v>
+        <v>38.121292169999997</v>
       </c>
       <c r="D244" s="30">
-        <v>-121.7090585</v>
+        <v>-122.0067224</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5348,13 +5386,13 @@
         <v>391</v>
       </c>
       <c r="B245" s="30" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C245" s="30">
-        <v>38.082940000000001</v>
+        <v>38.181780430000003</v>
       </c>
       <c r="D245" s="30">
-        <v>-121.72507</v>
+        <v>-121.91393739999999</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5362,13 +5400,13 @@
         <v>391</v>
       </c>
       <c r="B246" s="30" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C246" s="30">
-        <v>38.259950000000003</v>
+        <v>38.043095299999997</v>
       </c>
       <c r="D246" s="30">
-        <v>-121.79259999999999</v>
+        <v>-121.7992028</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5376,13 +5414,13 @@
         <v>391</v>
       </c>
       <c r="B247" s="30" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C247" s="30">
-        <v>38.243549999999999</v>
+        <v>38.08988506</v>
       </c>
       <c r="D247" s="30">
-        <v>-121.68453</v>
+        <v>-121.7090585</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5390,13 +5428,13 @@
         <v>391</v>
       </c>
       <c r="B248" s="30" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C248" s="30">
-        <v>38.242464470000002</v>
+        <v>38.082940000000001</v>
       </c>
       <c r="D248" s="30">
-        <v>-121.6618801</v>
+        <v>-121.72507</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5404,13 +5442,13 @@
         <v>391</v>
       </c>
       <c r="B249" s="30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C249" s="30">
-        <v>38.258112920000002</v>
+        <v>38.259950000000003</v>
       </c>
       <c r="D249" s="30">
-        <v>-121.653526</v>
+        <v>-121.79259999999999</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5418,13 +5456,13 @@
         <v>391</v>
       </c>
       <c r="B250" s="30" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C250" s="30">
-        <v>38.042189569999998</v>
+        <v>38.243549999999999</v>
       </c>
       <c r="D250" s="30">
-        <v>-121.84445169999999</v>
+        <v>-121.68453</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5432,13 +5470,13 @@
         <v>391</v>
       </c>
       <c r="B251" s="30" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C251" s="30">
-        <v>38.265309999999999</v>
+        <v>38.242464470000002</v>
       </c>
       <c r="D251" s="30">
-        <v>-121.78379</v>
+        <v>-121.6618801</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5446,13 +5484,13 @@
         <v>391</v>
       </c>
       <c r="B252" s="30" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C252" s="30">
-        <v>38.267819490000001</v>
+        <v>38.258112920000002</v>
       </c>
       <c r="D252" s="30">
-        <v>-121.7898314</v>
+        <v>-121.653526</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5460,13 +5498,13 @@
         <v>391</v>
       </c>
       <c r="B253" s="30" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C253" s="30">
-        <v>38.263213780000001</v>
+        <v>38.042189569999998</v>
       </c>
       <c r="D253" s="30">
-        <v>-121.7803662</v>
+        <v>-121.84445169999999</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5474,13 +5512,13 @@
         <v>391</v>
       </c>
       <c r="B254" s="30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C254" s="30">
-        <v>38.180309999999999</v>
+        <v>38.265309999999999</v>
       </c>
       <c r="D254" s="30">
-        <v>-121.90877999999999</v>
+        <v>-121.78379</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5488,13 +5526,13 @@
         <v>391</v>
       </c>
       <c r="B255" s="30" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C255" s="30">
-        <v>38.182479999999998</v>
+        <v>38.267819490000001</v>
       </c>
       <c r="D255" s="30">
-        <v>-121.92171999999999</v>
+        <v>-121.7898314</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5502,13 +5540,13 @@
         <v>391</v>
       </c>
       <c r="B256" s="30" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C256" s="30">
-        <v>38.039000000000001</v>
+        <v>38.263213780000001</v>
       </c>
       <c r="D256" s="30">
-        <v>-121.85760999999999</v>
+        <v>-121.7803662</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5516,13 +5554,13 @@
         <v>391</v>
       </c>
       <c r="B257" s="30" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C257" s="30">
-        <v>38.040502709999998</v>
+        <v>38.180309999999999</v>
       </c>
       <c r="D257" s="30">
-        <v>-121.8675863</v>
+        <v>-121.90877999999999</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5530,13 +5568,13 @@
         <v>391</v>
       </c>
       <c r="B258" s="30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C258" s="30">
-        <v>38.038130160000001</v>
+        <v>38.182479999999998</v>
       </c>
       <c r="D258" s="30">
-        <v>-121.8577899</v>
+        <v>-121.92171999999999</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5544,13 +5582,13 @@
         <v>391</v>
       </c>
       <c r="B259" s="30" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C259" s="30">
-        <v>38.286009999999997</v>
+        <v>38.039000000000001</v>
       </c>
       <c r="D259" s="30">
-        <v>-121.72101000000001</v>
+        <v>-121.85760999999999</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5558,23 +5596,27 @@
         <v>391</v>
       </c>
       <c r="B260" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C260" s="30"/>
-      <c r="D260" s="30"/>
+        <v>269</v>
+      </c>
+      <c r="C260" s="30">
+        <v>38.040502709999998</v>
+      </c>
+      <c r="D260" s="30">
+        <v>-121.8675863</v>
+      </c>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B261" s="30" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C261" s="30">
-        <v>38.26030111</v>
+        <v>38.038130160000001</v>
       </c>
       <c r="D261" s="30">
-        <v>-121.7811813</v>
+        <v>-121.8577899</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -5582,13 +5624,13 @@
         <v>391</v>
       </c>
       <c r="B262" s="30" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C262" s="30">
-        <v>38.259959870000003</v>
+        <v>38.286009999999997</v>
       </c>
       <c r="D262" s="30">
-        <v>-121.7906483</v>
+        <v>-121.72101000000001</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5596,27 +5638,23 @@
         <v>391</v>
       </c>
       <c r="B263" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="C263" s="30">
-        <v>38.083607880000002</v>
-      </c>
-      <c r="D263" s="30">
-        <v>-121.723387</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="C263" s="30"/>
+      <c r="D263" s="30"/>
     </row>
     <row r="264" spans="1:4">
       <c r="A264" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B264" s="30" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C264" s="30">
-        <v>38.10404278</v>
+        <v>38.26030111</v>
       </c>
       <c r="D264" s="30">
-        <v>-121.710669</v>
+        <v>-121.7811813</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5624,13 +5662,13 @@
         <v>391</v>
       </c>
       <c r="B265" s="30" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C265" s="30">
-        <v>38.09872661</v>
+        <v>38.259959870000003</v>
       </c>
       <c r="D265" s="30">
-        <v>-121.7090939</v>
+        <v>-121.7906483</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5638,13 +5676,13 @@
         <v>391</v>
       </c>
       <c r="B266" s="30" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C266" s="30">
-        <v>38.096895789999998</v>
+        <v>38.083607880000002</v>
       </c>
       <c r="D266" s="30">
-        <v>-121.7092772</v>
+        <v>-121.723387</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5652,13 +5690,13 @@
         <v>391</v>
       </c>
       <c r="B267" s="30" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C267" s="30">
-        <v>38.085120000000003</v>
+        <v>38.10404278</v>
       </c>
       <c r="D267" s="30">
-        <v>-121.72336</v>
+        <v>-121.710669</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -5666,13 +5704,13 @@
         <v>391</v>
       </c>
       <c r="B268" s="30" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C268" s="30">
-        <v>38.023244210000001</v>
+        <v>38.09872661</v>
       </c>
       <c r="D268" s="30">
-        <v>-121.8333619</v>
+        <v>-121.7090939</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5680,13 +5718,13 @@
         <v>391</v>
       </c>
       <c r="B269" s="30" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C269" s="30">
-        <v>38.021912989999997</v>
+        <v>38.096895789999998</v>
       </c>
       <c r="D269" s="30">
-        <v>-121.82532620000001</v>
+        <v>-121.7092772</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5694,13 +5732,13 @@
         <v>391</v>
       </c>
       <c r="B270" s="30" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C270" s="30">
-        <v>38.022789410000001</v>
+        <v>38.085120000000003</v>
       </c>
       <c r="D270" s="30">
-        <v>-121.8294301</v>
+        <v>-121.72336</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5708,13 +5746,13 @@
         <v>391</v>
       </c>
       <c r="B271" s="30" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C271" s="30">
-        <v>38.021887560000003</v>
+        <v>38.023244210000001</v>
       </c>
       <c r="D271" s="30">
-        <v>-121.83369709999999</v>
+        <v>-121.8333619</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5722,13 +5760,13 @@
         <v>391</v>
       </c>
       <c r="B272" s="30" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C272" s="30">
-        <v>38.023757349999997</v>
+        <v>38.021912989999997</v>
       </c>
       <c r="D272" s="30">
-        <v>-121.8272565</v>
+        <v>-121.82532620000001</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5736,13 +5774,13 @@
         <v>391</v>
       </c>
       <c r="B273" s="30" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C273" s="30">
-        <v>38.024821000000003</v>
+        <v>38.022789410000001</v>
       </c>
       <c r="D273" s="30">
-        <v>-121.82608999999999</v>
+        <v>-121.8294301</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5750,13 +5788,13 @@
         <v>391</v>
       </c>
       <c r="B274" s="30" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C274" s="30">
-        <v>38.295859999999998</v>
+        <v>38.021887560000003</v>
       </c>
       <c r="D274" s="30">
-        <v>-121.68886000000001</v>
+        <v>-121.83369709999999</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5764,13 +5802,13 @@
         <v>391</v>
       </c>
       <c r="B275" s="30" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C275" s="30">
-        <v>38.296002000000001</v>
+        <v>38.023757349999997</v>
       </c>
       <c r="D275" s="30">
-        <v>-121.68651800000001</v>
+        <v>-121.8272565</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5778,13 +5816,13 @@
         <v>391</v>
       </c>
       <c r="B276" s="30" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C276" s="30">
-        <v>38.364139999999999</v>
+        <v>38.024821000000003</v>
       </c>
       <c r="D276" s="30">
-        <v>-121.6444767</v>
+        <v>-121.82608999999999</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5792,13 +5830,13 @@
         <v>391</v>
       </c>
       <c r="B277" s="30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C277" s="30">
-        <v>38.03228</v>
+        <v>38.295859999999998</v>
       </c>
       <c r="D277" s="30">
-        <v>-121.47833</v>
+        <v>-121.68886000000001</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -5806,13 +5844,13 @@
         <v>391</v>
       </c>
       <c r="B278" s="30" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C278" s="30">
-        <v>38.082587820000001</v>
+        <v>38.296002000000001</v>
       </c>
       <c r="D278" s="30">
-        <v>-121.72807760000001</v>
+        <v>-121.68651800000001</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5820,13 +5858,13 @@
         <v>391</v>
       </c>
       <c r="B279" s="30" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C279" s="30">
-        <v>38.084034219999999</v>
+        <v>38.364139999999999</v>
       </c>
       <c r="D279" s="30">
-        <v>-121.7146892</v>
+        <v>-121.6444767</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5834,13 +5872,13 @@
         <v>391</v>
       </c>
       <c r="B280" s="30" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C280" s="30">
-        <v>38.099297280000002</v>
+        <v>38.03228</v>
       </c>
       <c r="D280" s="30">
-        <v>-121.7079337</v>
+        <v>-121.47833</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5848,13 +5886,13 @@
         <v>391</v>
       </c>
       <c r="B281" s="30" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C281" s="30">
-        <v>38.303673269999997</v>
+        <v>38.082587820000001</v>
       </c>
       <c r="D281" s="30">
-        <v>-121.7312177</v>
+        <v>-121.72807760000001</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5862,13 +5900,13 @@
         <v>391</v>
       </c>
       <c r="B282" s="30" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C282" s="30">
-        <v>38.277729919999999</v>
+        <v>38.084034219999999</v>
       </c>
       <c r="D282" s="30">
-        <v>-121.71053860000001</v>
+        <v>-121.7146892</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5876,13 +5914,13 @@
         <v>391</v>
       </c>
       <c r="B283" s="30" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C283" s="30">
-        <v>38.242040000000003</v>
+        <v>38.099297280000002</v>
       </c>
       <c r="D283" s="30">
-        <v>-121.68239</v>
+        <v>-121.7079337</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5890,13 +5928,13 @@
         <v>391</v>
       </c>
       <c r="B284" s="30" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C284" s="30">
-        <v>38.277189999999997</v>
+        <v>38.303673269999997</v>
       </c>
       <c r="D284" s="30">
-        <v>-121.69405999999999</v>
+        <v>-121.7312177</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5904,13 +5942,13 @@
         <v>391</v>
       </c>
       <c r="B285" s="30" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C285" s="30">
-        <v>38.246361999999998</v>
+        <v>38.277729919999999</v>
       </c>
       <c r="D285" s="30">
-        <v>-121.678139</v>
+        <v>-121.71053860000001</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5918,13 +5956,13 @@
         <v>391</v>
       </c>
       <c r="B286" s="30" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C286" s="30">
-        <v>38.269292</v>
+        <v>38.242040000000003</v>
       </c>
       <c r="D286" s="30">
-        <v>-121.691395</v>
+        <v>-121.68239</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5932,13 +5970,13 @@
         <v>391</v>
       </c>
       <c r="B287" s="30" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C287" s="30">
-        <v>38.255043000000001</v>
+        <v>38.277189999999997</v>
       </c>
       <c r="D287" s="30">
-        <v>-121.672072</v>
+        <v>-121.69405999999999</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5946,13 +5984,13 @@
         <v>391</v>
       </c>
       <c r="B288" s="30" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C288" s="30">
-        <v>38.257888000000001</v>
+        <v>38.246361999999998</v>
       </c>
       <c r="D288" s="30">
-        <v>-121.690273</v>
+        <v>-121.678139</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5960,13 +5998,13 @@
         <v>391</v>
       </c>
       <c r="B289" s="30" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C289" s="30">
-        <v>38.265140000000002</v>
+        <v>38.269292</v>
       </c>
       <c r="D289" s="30">
-        <v>-121.67155700000001</v>
+        <v>-121.691395</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5974,13 +6012,13 @@
         <v>391</v>
       </c>
       <c r="B290" s="30" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C290" s="30">
-        <v>38.252679999999998</v>
+        <v>38.255043000000001</v>
       </c>
       <c r="D290" s="30">
-        <v>-121.686263</v>
+        <v>-121.672072</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5988,13 +6026,13 @@
         <v>391</v>
       </c>
       <c r="B291" s="30" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C291" s="30">
-        <v>38.273775000000001</v>
+        <v>38.257888000000001</v>
       </c>
       <c r="D291" s="30">
-        <v>-121.66692999999999</v>
+        <v>-121.690273</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -6002,13 +6040,13 @@
         <v>391</v>
       </c>
       <c r="B292" s="30" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C292" s="30">
-        <v>38.244607000000002</v>
+        <v>38.265140000000002</v>
       </c>
       <c r="D292" s="30">
-        <v>-121.686421</v>
+        <v>-121.67155700000001</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -6016,13 +6054,13 @@
         <v>391</v>
       </c>
       <c r="B293" s="30" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C293" s="30">
-        <v>38.282319999999999</v>
+        <v>38.252679999999998</v>
       </c>
       <c r="D293" s="30">
-        <v>-121.69229</v>
+        <v>-121.686263</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6030,13 +6068,13 @@
         <v>391</v>
       </c>
       <c r="B294" s="30" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C294" s="30">
-        <v>38.284170000000003</v>
+        <v>38.273775000000001</v>
       </c>
       <c r="D294" s="30">
-        <v>-121.66531999999999</v>
+        <v>-121.66692999999999</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -6044,13 +6082,13 @@
         <v>391</v>
       </c>
       <c r="B295" s="30" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C295" s="30">
-        <v>38.288989999999998</v>
+        <v>38.244607000000002</v>
       </c>
       <c r="D295" s="30">
-        <v>-121.66651</v>
+        <v>-121.686421</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -6058,13 +6096,13 @@
         <v>391</v>
       </c>
       <c r="B296" s="30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C296" s="30">
-        <v>38.287590000000002</v>
+        <v>38.282319999999999</v>
       </c>
       <c r="D296" s="30">
-        <v>-121.69197</v>
+        <v>-121.69229</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -6072,13 +6110,13 @@
         <v>391</v>
       </c>
       <c r="B297" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C297" s="30">
-        <v>38.29607</v>
+        <v>38.284170000000003</v>
       </c>
       <c r="D297" s="30">
-        <v>-121.69193</v>
+        <v>-121.66531999999999</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -6086,13 +6124,13 @@
         <v>391</v>
       </c>
       <c r="B298" s="30" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C298" s="30">
-        <v>38.278500000000001</v>
+        <v>38.288989999999998</v>
       </c>
       <c r="D298" s="30">
-        <v>-121.69401999999999</v>
+        <v>-121.66651</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -6100,13 +6138,13 @@
         <v>391</v>
       </c>
       <c r="B299" s="30" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C299" s="30">
-        <v>38.290030000000002</v>
+        <v>38.287590000000002</v>
       </c>
       <c r="D299" s="30">
-        <v>-121.6918</v>
+        <v>-121.69197</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -6114,13 +6152,13 @@
         <v>391</v>
       </c>
       <c r="B300" s="30" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C300" s="30">
-        <v>38.296169999999996</v>
+        <v>38.29607</v>
       </c>
       <c r="D300" s="30">
-        <v>-121.68986</v>
+        <v>-121.69193</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -6128,13 +6166,13 @@
         <v>391</v>
       </c>
       <c r="B301" s="30" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C301" s="30">
-        <v>38.269620000000003</v>
+        <v>38.278500000000001</v>
       </c>
       <c r="D301" s="30">
-        <v>-121.67718000000001</v>
+        <v>-121.69401999999999</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -6142,13 +6180,13 @@
         <v>391</v>
       </c>
       <c r="B302" s="30" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C302" s="30">
-        <v>38.275649999999999</v>
+        <v>38.290030000000002</v>
       </c>
       <c r="D302" s="30">
-        <v>-121.67599</v>
+        <v>-121.6918</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6156,13 +6194,13 @@
         <v>391</v>
       </c>
       <c r="B303" s="30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C303" s="30">
-        <v>38.249670000000002</v>
+        <v>38.296169999999996</v>
       </c>
       <c r="D303" s="30">
-        <v>-121.67701</v>
+        <v>-121.68986</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -6170,13 +6208,13 @@
         <v>391</v>
       </c>
       <c r="B304" s="30" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C304" s="30">
-        <v>38.247709999999998</v>
+        <v>38.269620000000003</v>
       </c>
       <c r="D304" s="30">
-        <v>-121.67861000000001</v>
+        <v>-121.67718000000001</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6184,13 +6222,13 @@
         <v>391</v>
       </c>
       <c r="B305" s="30" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C305" s="30">
-        <v>38.26238</v>
+        <v>38.275649999999999</v>
       </c>
       <c r="D305" s="30">
-        <v>-121.67883</v>
+        <v>-121.67599</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6198,13 +6236,13 @@
         <v>391</v>
       </c>
       <c r="B306" s="30" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C306" s="30">
-        <v>38.267040000000001</v>
+        <v>38.249670000000002</v>
       </c>
       <c r="D306" s="30">
-        <v>-121.6879</v>
+        <v>-121.67701</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6212,13 +6250,13 @@
         <v>391</v>
       </c>
       <c r="B307" s="30" t="s">
-        <v>396</v>
+        <v>316</v>
       </c>
       <c r="C307" s="30">
-        <v>38.258663110000001</v>
+        <v>38.247709999999998</v>
       </c>
       <c r="D307" s="30">
-        <v>-121.79256650000001</v>
+        <v>-121.67861000000001</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -6226,13 +6264,13 @@
         <v>391</v>
       </c>
       <c r="B308" s="30" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C308" s="30">
-        <v>38.259518229999998</v>
+        <v>38.26238</v>
       </c>
       <c r="D308" s="30">
-        <v>-121.79754749999999</v>
+        <v>-121.67883</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -6240,13 +6278,13 @@
         <v>391</v>
       </c>
       <c r="B309" s="30" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C309" s="30">
-        <v>38.259779999999999</v>
+        <v>38.267040000000001</v>
       </c>
       <c r="D309" s="30">
-        <v>-121.7923</v>
+        <v>-121.6879</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -6254,13 +6292,13 @@
         <v>391</v>
       </c>
       <c r="B310" s="30" t="s">
-        <v>321</v>
+        <v>396</v>
       </c>
       <c r="C310" s="30">
-        <v>38.25902</v>
+        <v>38.258663110000001</v>
       </c>
       <c r="D310" s="30">
-        <v>-121.79259</v>
+        <v>-121.79256650000001</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6268,13 +6306,13 @@
         <v>391</v>
       </c>
       <c r="B311" s="30" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C311" s="30">
-        <v>38.260269030000003</v>
+        <v>38.259518229999998</v>
       </c>
       <c r="D311" s="30">
-        <v>-121.7616752</v>
+        <v>-121.79754749999999</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6282,13 +6320,13 @@
         <v>391</v>
       </c>
       <c r="B312" s="30" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C312" s="30">
-        <v>38.258149009999997</v>
+        <v>38.259779999999999</v>
       </c>
       <c r="D312" s="30">
-        <v>-121.73812100000001</v>
+        <v>-121.7923</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6296,13 +6334,13 @@
         <v>391</v>
       </c>
       <c r="B313" s="30" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C313" s="30">
-        <v>38.249980829999998</v>
+        <v>38.25902</v>
       </c>
       <c r="D313" s="30">
-        <v>-121.713593</v>
+        <v>-121.79259</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6310,13 +6348,13 @@
         <v>391</v>
       </c>
       <c r="B314" s="30" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C314" s="30">
-        <v>38.242319999999999</v>
+        <v>38.260269030000003</v>
       </c>
       <c r="D314" s="30">
-        <v>-121.66168</v>
+        <v>-121.7616752</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6324,13 +6362,13 @@
         <v>391</v>
       </c>
       <c r="B315" s="30" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C315" s="30">
-        <v>38.256869999999999</v>
+        <v>38.258149009999997</v>
       </c>
       <c r="D315" s="30">
-        <v>-121.6527</v>
+        <v>-121.73812100000001</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6338,13 +6376,13 @@
         <v>391</v>
       </c>
       <c r="B316" s="30" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C316" s="30">
-        <v>38.234140869999997</v>
+        <v>38.249980829999998</v>
       </c>
       <c r="D316" s="30">
-        <v>-121.6691908</v>
+        <v>-121.713593</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -6352,13 +6390,13 @@
         <v>391</v>
       </c>
       <c r="B317" s="30" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C317" s="30">
-        <v>38.24640849</v>
+        <v>38.242319999999999</v>
       </c>
       <c r="D317" s="30">
-        <v>-121.6595325</v>
+        <v>-121.66168</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -6366,13 +6404,13 @@
         <v>391</v>
       </c>
       <c r="B318" s="30" t="s">
-        <v>394</v>
+        <v>326</v>
       </c>
       <c r="C318" s="30">
-        <v>38.263632440000002</v>
+        <v>38.256869999999999</v>
       </c>
       <c r="D318" s="30">
-        <v>-121.6470267</v>
+        <v>-121.6527</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6380,13 +6418,13 @@
         <v>391</v>
       </c>
       <c r="B319" s="30" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C319" s="30">
-        <v>38.279973130000002</v>
+        <v>38.234140869999997</v>
       </c>
       <c r="D319" s="30">
-        <v>-121.64155239999999</v>
+        <v>-121.6691908</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -6394,13 +6432,13 @@
         <v>391</v>
       </c>
       <c r="B320" s="30" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C320" s="30">
-        <v>38.291833349999997</v>
+        <v>38.24640849</v>
       </c>
       <c r="D320" s="30">
-        <v>-121.6732488</v>
+        <v>-121.6595325</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -6408,13 +6446,13 @@
         <v>391</v>
       </c>
       <c r="B321" s="30" t="s">
-        <v>331</v>
+        <v>394</v>
       </c>
       <c r="C321" s="30">
-        <v>38.192741210000001</v>
+        <v>38.263632440000002</v>
       </c>
       <c r="D321" s="30">
-        <v>-121.92653540000001</v>
+        <v>-121.6470267</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -6422,13 +6460,13 @@
         <v>391</v>
       </c>
       <c r="B322" s="30" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C322" s="30">
-        <v>38.293072469999998</v>
+        <v>38.279973130000002</v>
       </c>
       <c r="D322" s="30">
-        <v>-121.6861237</v>
+        <v>-121.64155239999999</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6436,13 +6474,13 @@
         <v>391</v>
       </c>
       <c r="B323" s="30" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C323" s="30">
-        <v>38.24394144</v>
+        <v>38.291833349999997</v>
       </c>
       <c r="D323" s="30">
-        <v>-121.66362479999999</v>
+        <v>-121.6732488</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -6450,13 +6488,13 @@
         <v>391</v>
       </c>
       <c r="B324" s="30" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C324" s="30">
-        <v>38.31306549</v>
+        <v>38.192741210000001</v>
       </c>
       <c r="D324" s="30">
-        <v>-121.66714140000001</v>
+        <v>-121.92653540000001</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6464,13 +6502,13 @@
         <v>391</v>
       </c>
       <c r="B325" s="30" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C325" s="30">
-        <v>38.081829999999997</v>
+        <v>38.293072469999998</v>
       </c>
       <c r="D325" s="30">
-        <v>-121.72399</v>
+        <v>-121.6861237</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -6478,13 +6516,13 @@
         <v>391</v>
       </c>
       <c r="B326" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C326" s="30">
-        <v>38.083069999999999</v>
+        <v>38.24394144</v>
       </c>
       <c r="D326" s="30">
-        <v>-121.72206</v>
+        <v>-121.66362479999999</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -6492,13 +6530,13 @@
         <v>391</v>
       </c>
       <c r="B327" s="30" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C327" s="30">
-        <v>38.08558</v>
+        <v>38.31306549</v>
       </c>
       <c r="D327" s="30">
-        <v>-121.70901000000001</v>
+        <v>-121.66714140000001</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -6506,13 +6544,13 @@
         <v>391</v>
       </c>
       <c r="B328" s="30" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C328" s="30">
-        <v>38.08766</v>
+        <v>38.081829999999997</v>
       </c>
       <c r="D328" s="30">
-        <v>-121.71127</v>
+        <v>-121.72399</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6520,13 +6558,13 @@
         <v>391</v>
       </c>
       <c r="B329" s="30" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C329" s="30">
-        <v>38.10013</v>
+        <v>38.083069999999999</v>
       </c>
       <c r="D329" s="30">
-        <v>-121.70862</v>
+        <v>-121.72206</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -6534,13 +6572,13 @@
         <v>391</v>
       </c>
       <c r="B330" s="30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C330" s="30">
-        <v>38.100540000000002</v>
+        <v>38.08558</v>
       </c>
       <c r="D330" s="30">
-        <v>-121.70925</v>
+        <v>-121.70901000000001</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6548,13 +6586,13 @@
         <v>391</v>
       </c>
       <c r="B331" s="30" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C331" s="30">
-        <v>38.080979999999997</v>
+        <v>38.08766</v>
       </c>
       <c r="D331" s="30">
-        <v>-122.01718</v>
+        <v>-121.71127</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -6562,13 +6600,13 @@
         <v>391</v>
       </c>
       <c r="B332" s="30" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C332" s="30">
-        <v>38.085477750000003</v>
+        <v>38.10013</v>
       </c>
       <c r="D332" s="30">
-        <v>-122.01881400000001</v>
+        <v>-121.70862</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -6576,13 +6614,13 @@
         <v>391</v>
       </c>
       <c r="B333" s="30" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C333" s="30">
-        <v>38.083220560000001</v>
+        <v>38.100540000000002</v>
       </c>
       <c r="D333" s="30">
-        <v>-122.0083422</v>
+        <v>-121.70925</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -6590,13 +6628,13 @@
         <v>391</v>
       </c>
       <c r="B334" s="30" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C334" s="30">
-        <v>38.077246090000003</v>
+        <v>38.080979999999997</v>
       </c>
       <c r="D334" s="30">
-        <v>-122.0136547</v>
+        <v>-122.01718</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6604,13 +6642,13 @@
         <v>391</v>
       </c>
       <c r="B335" s="30" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C335" s="30">
-        <v>38.077816849999998</v>
+        <v>38.085477750000003</v>
       </c>
       <c r="D335" s="30">
-        <v>-122.00347290000001</v>
+        <v>-122.01881400000001</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -6618,13 +6656,13 @@
         <v>391</v>
       </c>
       <c r="B336" s="30" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C336" s="30">
-        <v>38.259108210000001</v>
+        <v>38.083220560000001</v>
       </c>
       <c r="D336" s="30">
-        <v>-121.677316</v>
+        <v>-122.0083422</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -6632,13 +6670,13 @@
         <v>391</v>
       </c>
       <c r="B337" s="30" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C337" s="30">
-        <v>38.279969999999999</v>
+        <v>38.077246090000003</v>
       </c>
       <c r="D337" s="30">
-        <v>-121.69346</v>
+        <v>-122.0136547</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -6646,13 +6684,13 @@
         <v>391</v>
       </c>
       <c r="B338" s="30" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C338" s="30">
-        <v>38.309820799999997</v>
+        <v>38.077816849999998</v>
       </c>
       <c r="D338" s="30">
-        <v>-121.6928649</v>
+        <v>-122.00347290000001</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -6660,13 +6698,13 @@
         <v>391</v>
       </c>
       <c r="B339" s="30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C339" s="30">
-        <v>38.278499140000001</v>
+        <v>38.259108210000001</v>
       </c>
       <c r="D339" s="30">
-        <v>-121.6934933</v>
+        <v>-121.677316</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -6674,13 +6712,13 @@
         <v>391</v>
       </c>
       <c r="B340" s="30" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C340" s="30">
-        <v>38.032170000000001</v>
+        <v>38.279969999999999</v>
       </c>
       <c r="D340" s="30">
-        <v>-121.47817000000001</v>
+        <v>-121.69346</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -6688,13 +6726,13 @@
         <v>391</v>
       </c>
       <c r="B341" s="30" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C341" s="30">
-        <v>38.03201</v>
+        <v>38.309820799999997</v>
       </c>
       <c r="D341" s="30">
-        <v>-121.47786000000001</v>
+        <v>-121.6928649</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6702,13 +6740,13 @@
         <v>391</v>
       </c>
       <c r="B342" s="30" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C342" s="30">
-        <v>38.009160000000001</v>
+        <v>38.278499140000001</v>
       </c>
       <c r="D342" s="30">
-        <v>-121.45679</v>
+        <v>-121.6934933</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -6716,13 +6754,13 @@
         <v>391</v>
       </c>
       <c r="B343" s="30" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C343" s="30">
-        <v>38.008040000000001</v>
+        <v>38.032170000000001</v>
       </c>
       <c r="D343" s="30">
-        <v>-121.45610000000001</v>
+        <v>-121.47817000000001</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -6730,13 +6768,13 @@
         <v>391</v>
       </c>
       <c r="B344" s="30" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C344" s="30">
-        <v>38.003909999999998</v>
+        <v>38.03201</v>
       </c>
       <c r="D344" s="30">
-        <v>-121.45036</v>
+        <v>-121.47786000000001</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -6744,13 +6782,13 @@
         <v>391</v>
       </c>
       <c r="B345" s="30" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C345" s="30">
-        <v>38.003450000000001</v>
+        <v>38.009160000000001</v>
       </c>
       <c r="D345" s="30">
-        <v>-121.45008</v>
+        <v>-121.45679</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -6758,13 +6796,13 @@
         <v>391</v>
       </c>
       <c r="B346" s="30" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C346" s="30">
-        <v>37.997709999999998</v>
+        <v>38.008040000000001</v>
       </c>
       <c r="D346" s="30">
-        <v>-121.44746000000001</v>
+        <v>-121.45610000000001</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -6772,13 +6810,13 @@
         <v>391</v>
       </c>
       <c r="B347" s="30" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C347" s="30">
-        <v>37.997520000000002</v>
+        <v>38.003909999999998</v>
       </c>
       <c r="D347" s="30">
-        <v>-121.44749</v>
+        <v>-121.45036</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6786,13 +6824,13 @@
         <v>391</v>
       </c>
       <c r="B348" s="30" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C348" s="30">
-        <v>38.249240190000002</v>
+        <v>38.003450000000001</v>
       </c>
       <c r="D348" s="30">
-        <v>-121.66372370000001</v>
+        <v>-121.45008</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6800,13 +6838,13 @@
         <v>391</v>
       </c>
       <c r="B349" s="30" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C349" s="30">
-        <v>38.244989259999997</v>
+        <v>37.997709999999998</v>
       </c>
       <c r="D349" s="30">
-        <v>-121.66946</v>
+        <v>-121.44746000000001</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6814,13 +6852,13 @@
         <v>391</v>
       </c>
       <c r="B350" s="30" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C350" s="30">
-        <v>38.238947359999997</v>
+        <v>37.997520000000002</v>
       </c>
       <c r="D350" s="30">
-        <v>-121.6687814</v>
+        <v>-121.44749</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6828,13 +6866,13 @@
         <v>391</v>
       </c>
       <c r="B351" s="30" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C351" s="30">
-        <v>38.251475419999998</v>
+        <v>38.249240190000002</v>
       </c>
       <c r="D351" s="30">
-        <v>-121.6603186</v>
+        <v>-121.66372370000001</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6842,10 +6880,10 @@
         <v>391</v>
       </c>
       <c r="B352" s="30" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C352" s="30">
-        <v>38.24192</v>
+        <v>38.244989259999997</v>
       </c>
       <c r="D352" s="30">
         <v>-121.66946</v>
@@ -6856,13 +6894,13 @@
         <v>391</v>
       </c>
       <c r="B353" s="30" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C353" s="30">
-        <v>38.237220000000001</v>
+        <v>38.238947359999997</v>
       </c>
       <c r="D353" s="30">
-        <v>-121.6692</v>
+        <v>-121.6687814</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6870,13 +6908,13 @@
         <v>391</v>
       </c>
       <c r="B354" s="30" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C354" s="30">
-        <v>38.245260629999997</v>
+        <v>38.251475419999998</v>
       </c>
       <c r="D354" s="30">
-        <v>-121.6604141</v>
+        <v>-121.6603186</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6884,23 +6922,27 @@
         <v>391</v>
       </c>
       <c r="B355" s="30" t="s">
-        <v>365</v>
-      </c>
-      <c r="C355" s="30"/>
-      <c r="D355" s="30"/>
+        <v>362</v>
+      </c>
+      <c r="C355" s="30">
+        <v>38.24192</v>
+      </c>
+      <c r="D355" s="30">
+        <v>-121.66946</v>
+      </c>
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B356" s="30" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C356" s="30">
-        <v>38.094700000000003</v>
+        <v>38.237220000000001</v>
       </c>
       <c r="D356" s="30">
-        <v>-121.59039</v>
+        <v>-121.6692</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6908,13 +6950,13 @@
         <v>391</v>
       </c>
       <c r="B357" s="30" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C357" s="30">
-        <v>38.326660760000003</v>
+        <v>38.245260629999997</v>
       </c>
       <c r="D357" s="30">
-        <v>-121.68302919999999</v>
+        <v>-121.6604141</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6922,27 +6964,23 @@
         <v>391</v>
       </c>
       <c r="B358" s="30" t="s">
-        <v>368</v>
-      </c>
-      <c r="C358" s="30">
-        <v>38.333898980000001</v>
-      </c>
-      <c r="D358" s="30">
-        <v>-121.6739171</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="C358" s="30"/>
+      <c r="D358" s="30"/>
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B359" s="30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C359" s="30">
-        <v>38.344457859999999</v>
+        <v>38.094700000000003</v>
       </c>
       <c r="D359" s="30">
-        <v>-121.6554718</v>
+        <v>-121.59039</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6950,13 +6988,13 @@
         <v>391</v>
       </c>
       <c r="B360" s="30" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C360" s="30">
-        <v>38.299759999999999</v>
+        <v>38.326660760000003</v>
       </c>
       <c r="D360" s="30">
-        <v>-121.68925</v>
+        <v>-121.68302919999999</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6964,13 +7002,13 @@
         <v>391</v>
       </c>
       <c r="B361" s="30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C361" s="30">
-        <v>38.299639999999997</v>
+        <v>38.333898980000001</v>
       </c>
       <c r="D361" s="30">
-        <v>-121.69061000000001</v>
+        <v>-121.6739171</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6978,13 +7016,13 @@
         <v>391</v>
       </c>
       <c r="B362" s="30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C362" s="30">
-        <v>38.261318639999999</v>
+        <v>38.344457859999999</v>
       </c>
       <c r="D362" s="30">
-        <v>-121.6860805</v>
+        <v>-121.6554718</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6992,13 +7030,13 @@
         <v>391</v>
       </c>
       <c r="B363" s="30" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C363" s="30">
-        <v>38.169350000000001</v>
+        <v>38.299759999999999</v>
       </c>
       <c r="D363" s="30">
-        <v>-121.41540999999999</v>
+        <v>-121.68925</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -7006,13 +7044,13 @@
         <v>391</v>
       </c>
       <c r="B364" s="30" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C364" s="30">
-        <v>38.356349690000002</v>
+        <v>38.299639999999997</v>
       </c>
       <c r="D364" s="30">
-        <v>-121.6418877</v>
+        <v>-121.69061000000001</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -7020,13 +7058,13 @@
         <v>391</v>
       </c>
       <c r="B365" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C365" s="30">
-        <v>38.120756800000002</v>
+        <v>38.261318639999999</v>
       </c>
       <c r="D365" s="30">
-        <v>-121.9818389</v>
+        <v>-121.6860805</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -7034,13 +7072,13 @@
         <v>391</v>
       </c>
       <c r="B366" s="30" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C366" s="30">
-        <v>38.122772070000003</v>
+        <v>38.169350000000001</v>
       </c>
       <c r="D366" s="30">
-        <v>-121.9860338</v>
+        <v>-121.41540999999999</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -7048,13 +7086,13 @@
         <v>391</v>
       </c>
       <c r="B367" s="30" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C367" s="30">
-        <v>38.128327800000001</v>
+        <v>38.356349690000002</v>
       </c>
       <c r="D367" s="30">
-        <v>-121.9895781</v>
+        <v>-121.6418877</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -7062,13 +7100,13 @@
         <v>391</v>
       </c>
       <c r="B368" s="30" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C368" s="30">
-        <v>38.134869999999999</v>
+        <v>38.120756800000002</v>
       </c>
       <c r="D368" s="30">
-        <v>-121.99668</v>
+        <v>-121.9818389</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -7076,13 +7114,13 @@
         <v>391</v>
       </c>
       <c r="B369" s="30" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C369" s="30">
-        <v>38.134869999999999</v>
+        <v>38.122772070000003</v>
       </c>
       <c r="D369" s="30">
-        <v>-121.99668</v>
+        <v>-121.9860338</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -7090,13 +7128,13 @@
         <v>391</v>
       </c>
       <c r="B370" s="30" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C370" s="30">
-        <v>38.113599999999998</v>
+        <v>38.128327800000001</v>
       </c>
       <c r="D370" s="30">
-        <v>-121.98169</v>
+        <v>-121.9895781</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -7104,13 +7142,13 @@
         <v>391</v>
       </c>
       <c r="B371" s="30" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C371" s="30">
-        <v>38.113779999999998</v>
+        <v>38.134869999999999</v>
       </c>
       <c r="D371" s="30">
-        <v>-121.98161</v>
+        <v>-121.99668</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -7118,13 +7156,13 @@
         <v>391</v>
       </c>
       <c r="B372" s="30" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C372" s="30">
-        <v>38.09502792</v>
+        <v>38.134869999999999</v>
       </c>
       <c r="D372" s="30">
-        <v>-121.5879041</v>
+        <v>-121.99668</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -7132,13 +7170,13 @@
         <v>391</v>
       </c>
       <c r="B373" s="30" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C373" s="30">
-        <v>38.334020000000002</v>
+        <v>38.113599999999998</v>
       </c>
       <c r="D373" s="30">
-        <v>-121.67107</v>
+        <v>-121.98169</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7146,13 +7184,13 @@
         <v>391</v>
       </c>
       <c r="B374" s="30" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="C374" s="30">
-        <v>38.045928529999998</v>
+        <v>38.113779999999998</v>
       </c>
       <c r="D374" s="30">
-        <v>-121.84750099999999</v>
+        <v>-121.98161</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7160,13 +7198,13 @@
         <v>391</v>
       </c>
       <c r="B375" s="30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C375" s="30">
-        <v>38.226939999999999</v>
+        <v>38.09502792</v>
       </c>
       <c r="D375" s="30">
-        <v>-122.03591</v>
+        <v>-121.5879041</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7174,13 +7212,13 @@
         <v>391</v>
       </c>
       <c r="B376" s="30" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C376" s="30">
-        <v>38.226010000000002</v>
+        <v>38.334020000000002</v>
       </c>
       <c r="D376" s="30">
-        <v>-122.03825999999999</v>
+        <v>-121.67107</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7188,13 +7226,13 @@
         <v>391</v>
       </c>
       <c r="B377" s="30" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C377" s="30">
-        <v>38.049653829999997</v>
+        <v>38.045928529999998</v>
       </c>
       <c r="D377" s="30">
-        <v>-121.8488996</v>
+        <v>-121.84750099999999</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7202,13 +7240,13 @@
         <v>391</v>
       </c>
       <c r="B378" s="30" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C378" s="30">
-        <v>38.037943380000002</v>
+        <v>38.226939999999999</v>
       </c>
       <c r="D378" s="30">
-        <v>-121.84428459999999</v>
+        <v>-122.03591</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7216,13 +7254,13 @@
         <v>391</v>
       </c>
       <c r="B379" s="30" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C379" s="30">
-        <v>38.030609779999999</v>
+        <v>38.226010000000002</v>
       </c>
       <c r="D379" s="30">
-        <v>-121.8414193</v>
+        <v>-122.03825999999999</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7230,13 +7268,13 @@
         <v>391</v>
       </c>
       <c r="B380" s="30" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C380" s="30">
-        <v>38.052289080000001</v>
+        <v>38.049653829999997</v>
       </c>
       <c r="D380" s="30">
-        <v>-121.85680499999999</v>
+        <v>-121.8488996</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7244,69 +7282,69 @@
         <v>391</v>
       </c>
       <c r="B381" s="30" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C381" s="30">
-        <v>38.052123680000001</v>
+        <v>38.037943380000002</v>
       </c>
       <c r="D381" s="30">
-        <v>-121.8542861</v>
+        <v>-121.84428459999999</v>
       </c>
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="B382" s="34" t="s">
-        <v>397</v>
-      </c>
-      <c r="C382" s="36">
-        <v>38.544499999999999</v>
-      </c>
-      <c r="D382" s="36">
-        <v>-121.58663900000001</v>
+        <v>391</v>
+      </c>
+      <c r="B382" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C382" s="30">
+        <v>38.030609779999999</v>
+      </c>
+      <c r="D382" s="30">
+        <v>-121.8414193</v>
       </c>
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="B383" s="35" t="s">
-        <v>398</v>
-      </c>
-      <c r="C383" s="37">
-        <v>38.528060000000004</v>
-      </c>
-      <c r="D383" s="37">
-        <v>-121.58663900000001</v>
+        <v>391</v>
+      </c>
+      <c r="B383" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="C383" s="30">
+        <v>38.052289080000001</v>
+      </c>
+      <c r="D383" s="30">
+        <v>-121.85680499999999</v>
       </c>
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="28" t="s">
-        <v>447</v>
-      </c>
-      <c r="B384" s="35" t="s">
-        <v>399</v>
-      </c>
-      <c r="C384" s="37">
-        <v>38.518500000000003</v>
-      </c>
-      <c r="D384" s="37">
-        <v>-121.588623</v>
+        <v>391</v>
+      </c>
+      <c r="B384" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="C384" s="30">
+        <v>38.052123680000001</v>
+      </c>
+      <c r="D384" s="30">
+        <v>-121.8542861</v>
       </c>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="28" t="s">
         <v>447</v>
       </c>
-      <c r="B385" s="35" t="s">
-        <v>400</v>
-      </c>
-      <c r="C385" s="37">
-        <v>38.494390000000003</v>
-      </c>
-      <c r="D385" s="37">
-        <v>-121.588583</v>
+      <c r="B385" s="34" t="s">
+        <v>397</v>
+      </c>
+      <c r="C385" s="36">
+        <v>38.544499999999999</v>
+      </c>
+      <c r="D385" s="36">
+        <v>-121.58663900000001</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -7314,13 +7352,13 @@
         <v>447</v>
       </c>
       <c r="B386" s="35" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C386" s="37">
-        <v>38.436971</v>
+        <v>38.528060000000004</v>
       </c>
       <c r="D386" s="37">
-        <v>-121.604878</v>
+        <v>-121.58663900000001</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -7328,13 +7366,13 @@
         <v>447</v>
       </c>
       <c r="B387" s="35" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C387" s="37">
-        <v>38.466810000000002</v>
+        <v>38.518500000000003</v>
       </c>
       <c r="D387" s="37">
-        <v>-121.590851</v>
+        <v>-121.588623</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -7342,13 +7380,13 @@
         <v>447</v>
       </c>
       <c r="B388" s="35" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C388" s="37">
-        <v>38.431890000000003</v>
+        <v>38.494390000000003</v>
       </c>
       <c r="D388" s="37">
-        <v>-121.60705299999999</v>
+        <v>-121.588583</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -7356,13 +7394,13 @@
         <v>447</v>
       </c>
       <c r="B389" s="35" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C389" s="37">
-        <v>38.389389999999999</v>
+        <v>38.436971</v>
       </c>
       <c r="D389" s="37">
-        <v>-121.626278</v>
+        <v>-121.604878</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -7370,13 +7408,13 @@
         <v>447</v>
       </c>
       <c r="B390" s="35" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C390" s="37">
-        <v>38.354959999999998</v>
+        <v>38.466810000000002</v>
       </c>
       <c r="D390" s="37">
-        <v>-121.6422</v>
+        <v>-121.590851</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -7384,13 +7422,13 @@
         <v>447</v>
       </c>
       <c r="B391" s="35" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C391" s="37">
-        <v>38.274279999999997</v>
+        <v>38.431890000000003</v>
       </c>
       <c r="D391" s="37">
-        <v>-121.66417800000001</v>
+        <v>-121.60705299999999</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -7398,13 +7436,13 @@
         <v>447</v>
       </c>
       <c r="B392" s="35" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C392" s="37">
-        <v>38.282465000000002</v>
+        <v>38.389389999999999</v>
       </c>
       <c r="D392" s="37">
-        <v>-121.66318200000001</v>
+        <v>-121.626278</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -7412,13 +7450,13 @@
         <v>447</v>
       </c>
       <c r="B393" s="35" t="s">
-        <v>408</v>
-      </c>
-      <c r="C393" s="38">
-        <v>38.355609999999999</v>
-      </c>
-      <c r="D393" s="38">
-        <v>-121.35257</v>
+        <v>405</v>
+      </c>
+      <c r="C393" s="37">
+        <v>38.354959999999998</v>
+      </c>
+      <c r="D393" s="37">
+        <v>-121.6422</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -7426,13 +7464,13 @@
         <v>447</v>
       </c>
       <c r="B394" s="35" t="s">
-        <v>409</v>
-      </c>
-      <c r="C394" s="38">
-        <v>38.364699999999999</v>
-      </c>
-      <c r="D394" s="38">
-        <v>-121.35596</v>
+        <v>406</v>
+      </c>
+      <c r="C394" s="37">
+        <v>38.274279999999997</v>
+      </c>
+      <c r="D394" s="37">
+        <v>-121.66417800000001</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -7440,13 +7478,13 @@
         <v>447</v>
       </c>
       <c r="B395" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="C395" s="38">
-        <v>38.371920000000003</v>
-      </c>
-      <c r="D395" s="38">
-        <v>-121.36291</v>
+        <v>407</v>
+      </c>
+      <c r="C395" s="37">
+        <v>38.282465000000002</v>
+      </c>
+      <c r="D395" s="37">
+        <v>-121.66318200000001</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -7454,13 +7492,13 @@
         <v>447</v>
       </c>
       <c r="B396" s="35" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C396" s="38">
-        <v>38.382579999999997</v>
+        <v>38.355609999999999</v>
       </c>
       <c r="D396" s="38">
-        <v>-121.37130999999999</v>
+        <v>-121.35257</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -7468,33 +7506,41 @@
         <v>447</v>
       </c>
       <c r="B397" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="C397" s="39"/>
-      <c r="D397" s="39"/>
+        <v>409</v>
+      </c>
+      <c r="C397" s="38">
+        <v>38.364699999999999</v>
+      </c>
+      <c r="D397" s="38">
+        <v>-121.35596</v>
+      </c>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B398" s="35" t="s">
-        <v>413</v>
-      </c>
-      <c r="C398" s="40"/>
-      <c r="D398" s="40"/>
+        <v>410</v>
+      </c>
+      <c r="C398" s="38">
+        <v>38.371920000000003</v>
+      </c>
+      <c r="D398" s="38">
+        <v>-121.36291</v>
+      </c>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B399" s="35" t="s">
-        <v>414</v>
-      </c>
-      <c r="C399" s="36">
-        <v>38.675919999999998</v>
-      </c>
-      <c r="D399" s="36">
-        <v>-121.64343599999999</v>
+        <v>411</v>
+      </c>
+      <c r="C399" s="38">
+        <v>38.382579999999997</v>
+      </c>
+      <c r="D399" s="38">
+        <v>-121.37130999999999</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -7502,41 +7548,33 @@
         <v>447</v>
       </c>
       <c r="B400" s="35" t="s">
-        <v>415</v>
-      </c>
-      <c r="C400" s="37">
-        <v>38.749789999999997</v>
-      </c>
-      <c r="D400" s="37">
-        <v>-121.635232</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="C400" s="39"/>
+      <c r="D400" s="39"/>
     </row>
     <row r="401" spans="1:4">
       <c r="A401" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B401" s="35" t="s">
-        <v>416</v>
-      </c>
-      <c r="C401" s="37">
-        <v>38.474170000000001</v>
-      </c>
-      <c r="D401" s="37">
-        <v>-121.588083</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="C401" s="40"/>
+      <c r="D401" s="40"/>
     </row>
     <row r="402" spans="1:4">
       <c r="A402" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B402" s="35" t="s">
-        <v>417</v>
-      </c>
-      <c r="C402" s="41">
-        <v>38.473550000000003</v>
-      </c>
-      <c r="D402" s="41">
-        <v>-121.588364</v>
+        <v>414</v>
+      </c>
+      <c r="C402" s="36">
+        <v>38.675919999999998</v>
+      </c>
+      <c r="D402" s="36">
+        <v>-121.64343599999999</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -7544,13 +7582,13 @@
         <v>447</v>
       </c>
       <c r="B403" s="35" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C403" s="37">
-        <v>38.466957999999998</v>
+        <v>38.749789999999997</v>
       </c>
       <c r="D403" s="37">
-        <v>-121.590934</v>
+        <v>-121.635232</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -7558,13 +7596,13 @@
         <v>447</v>
       </c>
       <c r="B404" s="35" t="s">
-        <v>419</v>
-      </c>
-      <c r="C404" s="41">
-        <v>38.676366999999999</v>
-      </c>
-      <c r="D404" s="41">
-        <v>-121.64397200000001</v>
+        <v>416</v>
+      </c>
+      <c r="C404" s="37">
+        <v>38.474170000000001</v>
+      </c>
+      <c r="D404" s="37">
+        <v>-121.588083</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -7572,13 +7610,13 @@
         <v>447</v>
       </c>
       <c r="B405" s="35" t="s">
-        <v>420</v>
-      </c>
-      <c r="C405" s="42">
-        <v>38.605218999999998</v>
-      </c>
-      <c r="D405" s="43">
-        <v>-121.564176</v>
+        <v>417</v>
+      </c>
+      <c r="C405" s="41">
+        <v>38.473550000000003</v>
+      </c>
+      <c r="D405" s="41">
+        <v>-121.588364</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -7586,37 +7624,49 @@
         <v>447</v>
       </c>
       <c r="B406" s="35" t="s">
-        <v>421</v>
-      </c>
-      <c r="C406" s="41"/>
-      <c r="D406" s="41"/>
+        <v>418</v>
+      </c>
+      <c r="C406" s="37">
+        <v>38.466957999999998</v>
+      </c>
+      <c r="D406" s="37">
+        <v>-121.590934</v>
+      </c>
     </row>
     <row r="407" spans="1:4">
       <c r="A407" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B407" s="35" t="s">
-        <v>422</v>
-      </c>
-      <c r="C407" s="44"/>
-      <c r="D407" s="44"/>
+        <v>419</v>
+      </c>
+      <c r="C407" s="41">
+        <v>38.676366999999999</v>
+      </c>
+      <c r="D407" s="41">
+        <v>-121.64397200000001</v>
+      </c>
     </row>
     <row r="408" spans="1:4">
       <c r="A408" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B408" s="35" t="s">
-        <v>423</v>
-      </c>
-      <c r="C408" s="44"/>
-      <c r="D408" s="44"/>
+        <v>420</v>
+      </c>
+      <c r="C408" s="42">
+        <v>38.605218999999998</v>
+      </c>
+      <c r="D408" s="43">
+        <v>-121.564176</v>
+      </c>
     </row>
     <row r="409" spans="1:4">
       <c r="A409" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B409" s="35" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C409" s="41"/>
       <c r="D409" s="41"/>
@@ -7626,55 +7676,43 @@
         <v>447</v>
       </c>
       <c r="B410" s="35" t="s">
-        <v>425</v>
-      </c>
-      <c r="C410" s="37">
-        <v>38.353383000000001</v>
-      </c>
-      <c r="D410" s="37">
-        <v>-121.643181</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="C410" s="44"/>
+      <c r="D410" s="44"/>
     </row>
     <row r="411" spans="1:4">
       <c r="A411" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B411" s="35" t="s">
-        <v>426</v>
-      </c>
-      <c r="C411" s="37">
-        <v>38.605218999999998</v>
-      </c>
-      <c r="D411" s="37">
-        <v>-121.564176</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="C411" s="44"/>
+      <c r="D411" s="44"/>
     </row>
     <row r="412" spans="1:4">
       <c r="A412" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B412" s="35" t="s">
-        <v>427</v>
-      </c>
-      <c r="C412" s="37">
-        <v>38.565379999999998</v>
-      </c>
-      <c r="D412" s="37">
-        <v>-121.630989</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="C412" s="41"/>
+      <c r="D412" s="41"/>
     </row>
     <row r="413" spans="1:4">
       <c r="A413" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B413" s="35" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C413" s="37">
-        <v>38.565309999999997</v>
+        <v>38.353383000000001</v>
       </c>
       <c r="D413" s="37">
-        <v>-121.63800500000001</v>
+        <v>-121.643181</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -7682,13 +7720,13 @@
         <v>447</v>
       </c>
       <c r="B414" s="35" t="s">
-        <v>429</v>
-      </c>
-      <c r="C414" s="36">
-        <v>38.675919999999998</v>
-      </c>
-      <c r="D414" s="36">
-        <v>-121.64343599999999</v>
+        <v>426</v>
+      </c>
+      <c r="C414" s="37">
+        <v>38.605218999999998</v>
+      </c>
+      <c r="D414" s="37">
+        <v>-121.564176</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -7696,13 +7734,13 @@
         <v>447</v>
       </c>
       <c r="B415" s="35" t="s">
-        <v>430</v>
-      </c>
-      <c r="C415" s="39">
-        <v>38.567056999999998</v>
-      </c>
-      <c r="D415" s="39">
-        <v>-121.638239</v>
+        <v>427</v>
+      </c>
+      <c r="C415" s="37">
+        <v>38.565379999999998</v>
+      </c>
+      <c r="D415" s="37">
+        <v>-121.630989</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -7710,13 +7748,13 @@
         <v>447</v>
       </c>
       <c r="B416" s="35" t="s">
-        <v>431</v>
-      </c>
-      <c r="C416" s="39">
-        <v>38.573110999999997</v>
-      </c>
-      <c r="D416" s="39">
-        <v>-121.582958</v>
+        <v>428</v>
+      </c>
+      <c r="C416" s="37">
+        <v>38.565309999999997</v>
+      </c>
+      <c r="D416" s="37">
+        <v>-121.63800500000001</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -7724,23 +7762,27 @@
         <v>447</v>
       </c>
       <c r="B417" s="35" t="s">
-        <v>432</v>
-      </c>
-      <c r="C417" s="39"/>
-      <c r="D417" s="39"/>
+        <v>429</v>
+      </c>
+      <c r="C417" s="36">
+        <v>38.675919999999998</v>
+      </c>
+      <c r="D417" s="36">
+        <v>-121.64343599999999</v>
+      </c>
     </row>
     <row r="418" spans="1:4">
       <c r="A418" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B418" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="C418" s="45">
-        <v>38.242100000000001</v>
-      </c>
-      <c r="D418" s="46">
-        <v>-121.6849</v>
+        <v>430</v>
+      </c>
+      <c r="C418" s="39">
+        <v>38.567056999999998</v>
+      </c>
+      <c r="D418" s="39">
+        <v>-121.638239</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -7748,13 +7790,13 @@
         <v>447</v>
       </c>
       <c r="B419" s="35" t="s">
-        <v>434</v>
-      </c>
-      <c r="C419" s="37">
-        <v>38.474815999999997</v>
-      </c>
-      <c r="D419" s="37">
-        <v>-121.588584</v>
+        <v>431</v>
+      </c>
+      <c r="C419" s="39">
+        <v>38.573110999999997</v>
+      </c>
+      <c r="D419" s="39">
+        <v>-121.582958</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -7762,27 +7804,23 @@
         <v>447</v>
       </c>
       <c r="B420" s="35" t="s">
-        <v>435</v>
-      </c>
-      <c r="C420" s="39">
-        <v>38.793456999999997</v>
-      </c>
-      <c r="D420" s="39">
-        <v>-121.725447</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="C420" s="39"/>
+      <c r="D420" s="39"/>
     </row>
     <row r="421" spans="1:4">
       <c r="A421" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B421" s="35" t="s">
-        <v>436</v>
-      </c>
-      <c r="C421" s="42">
-        <v>38.842001000000003</v>
-      </c>
-      <c r="D421" s="42">
-        <v>-121.85837100000001</v>
+        <v>433</v>
+      </c>
+      <c r="C421" s="45">
+        <v>38.242100000000001</v>
+      </c>
+      <c r="D421" s="46">
+        <v>-121.6849</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -7790,13 +7828,13 @@
         <v>447</v>
       </c>
       <c r="B422" s="35" t="s">
-        <v>437</v>
-      </c>
-      <c r="C422" s="39">
-        <v>38.159737</v>
-      </c>
-      <c r="D422" s="39">
-        <v>-121.68635500000001</v>
+        <v>434</v>
+      </c>
+      <c r="C422" s="37">
+        <v>38.474815999999997</v>
+      </c>
+      <c r="D422" s="37">
+        <v>-121.588584</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -7804,13 +7842,13 @@
         <v>447</v>
       </c>
       <c r="B423" s="35" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C423" s="39">
-        <v>38.213166999999999</v>
+        <v>38.793456999999997</v>
       </c>
       <c r="D423" s="39">
-        <v>-121.66859100000001</v>
+        <v>-121.725447</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -7818,13 +7856,13 @@
         <v>447</v>
       </c>
       <c r="B424" s="35" t="s">
-        <v>439</v>
-      </c>
-      <c r="C424" s="46">
-        <v>38.093400000000003</v>
-      </c>
-      <c r="D424" s="46">
-        <v>-121.736</v>
+        <v>436</v>
+      </c>
+      <c r="C424" s="42">
+        <v>38.842001000000003</v>
+      </c>
+      <c r="D424" s="42">
+        <v>-121.85837100000001</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -7832,13 +7870,13 @@
         <v>447</v>
       </c>
       <c r="B425" s="35" t="s">
-        <v>440</v>
-      </c>
-      <c r="C425" s="43">
-        <v>38.531880999999998</v>
-      </c>
-      <c r="D425" s="43">
-        <v>-121.527912</v>
+        <v>437</v>
+      </c>
+      <c r="C425" s="39">
+        <v>38.159737</v>
+      </c>
+      <c r="D425" s="39">
+        <v>-121.68635500000001</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -7846,23 +7884,27 @@
         <v>447</v>
       </c>
       <c r="B426" s="35" t="s">
-        <v>441</v>
-      </c>
-      <c r="C426" s="39"/>
-      <c r="D426" s="39"/>
+        <v>438</v>
+      </c>
+      <c r="C426" s="39">
+        <v>38.213166999999999</v>
+      </c>
+      <c r="D426" s="39">
+        <v>-121.66859100000001</v>
+      </c>
     </row>
     <row r="427" spans="1:4">
       <c r="A427" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B427" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="C427" s="39">
-        <v>38.681621</v>
-      </c>
-      <c r="D427" s="39">
-        <v>-121.645775</v>
+        <v>439</v>
+      </c>
+      <c r="C427" s="46">
+        <v>38.093400000000003</v>
+      </c>
+      <c r="D427" s="46">
+        <v>-121.736</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -7870,13 +7912,13 @@
         <v>447</v>
       </c>
       <c r="B428" s="35" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C428" s="43">
-        <v>38.47157</v>
-      </c>
-      <c r="D428" s="37">
-        <v>-121.63334999999999</v>
+        <v>38.531880999999998</v>
+      </c>
+      <c r="D428" s="43">
+        <v>-121.527912</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -7884,27 +7926,23 @@
         <v>447</v>
       </c>
       <c r="B429" s="35" t="s">
-        <v>444</v>
-      </c>
-      <c r="C429" s="43">
-        <v>38.470230000000001</v>
-      </c>
-      <c r="D429" s="47">
-        <v>-121.62105</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="C429" s="39"/>
+      <c r="D429" s="39"/>
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="28" t="s">
         <v>447</v>
       </c>
       <c r="B430" s="35" t="s">
-        <v>445</v>
-      </c>
-      <c r="C430" s="43">
-        <v>38.471620000000001</v>
-      </c>
-      <c r="D430" s="47">
-        <v>-121.60711999999999</v>
+        <v>442</v>
+      </c>
+      <c r="C430" s="39">
+        <v>38.681621</v>
+      </c>
+      <c r="D430" s="39">
+        <v>-121.645775</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -7912,12 +7950,54 @@
         <v>447</v>
       </c>
       <c r="B431" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="C431" s="43">
+        <v>38.47157</v>
+      </c>
+      <c r="D431" s="37">
+        <v>-121.63334999999999</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4">
+      <c r="A432" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B432" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="C432" s="43">
+        <v>38.470230000000001</v>
+      </c>
+      <c r="D432" s="47">
+        <v>-121.62105</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4">
+      <c r="A433" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B433" s="35" t="s">
+        <v>445</v>
+      </c>
+      <c r="C433" s="43">
+        <v>38.471620000000001</v>
+      </c>
+      <c r="D433" s="47">
+        <v>-121.60711999999999</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4">
+      <c r="A434" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="B434" s="35" t="s">
         <v>446</v>
       </c>
-      <c r="C431" s="43">
+      <c r="C434" s="43">
         <v>38.472580000000001</v>
       </c>
-      <c r="D431" s="47">
+      <c r="D434" s="47">
         <v>-121.59430999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added station location for FMWT 520 (=STN 520)
</commit_message>
<xml_diff>
--- a/data-raw/stations.xlsx
+++ b/data-raw/stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983EA3E5-B862-4A16-80B2-9AF2C317852E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EB61C1-2897-450E-B20B-C29E1FD531B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1857,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G394"/>
+  <dimension ref="A1:G393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A358" workbookViewId="0">
-      <selection activeCell="C390" sqref="C390"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="A347" sqref="A347:XFD347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6615,8 +6615,14 @@
       <c r="A347" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B347" s="28" t="s">
-        <v>210</v>
+      <c r="B347">
+        <v>340</v>
+      </c>
+      <c r="C347">
+        <v>38.105080000000001</v>
+      </c>
+      <c r="D347">
+        <v>-122.26988</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6624,13 +6630,13 @@
         <v>198</v>
       </c>
       <c r="B348">
-        <v>340</v>
+        <v>405</v>
       </c>
       <c r="C348">
-        <v>38.105080000000001</v>
+        <v>38.033529999999999</v>
       </c>
       <c r="D348">
-        <v>-122.26988</v>
+        <v>-122.15815000000001</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6638,13 +6644,13 @@
         <v>198</v>
       </c>
       <c r="B349">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="C349">
-        <v>38.033529999999999</v>
+        <v>38.061169999999997</v>
       </c>
       <c r="D349">
-        <v>-122.15815000000001</v>
+        <v>-122.06828</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6652,13 +6658,13 @@
         <v>198</v>
       </c>
       <c r="B350">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="C350">
-        <v>38.061169999999997</v>
+        <v>38.0702</v>
       </c>
       <c r="D350">
-        <v>-122.06828</v>
+        <v>-122.09415</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6666,13 +6672,13 @@
         <v>198</v>
       </c>
       <c r="B351">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C351">
-        <v>38.0702</v>
+        <v>38.093829999999997</v>
       </c>
       <c r="D351">
-        <v>-122.09415</v>
+        <v>-122.06973000000001</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6680,13 +6686,13 @@
         <v>198</v>
       </c>
       <c r="B352">
-        <v>418</v>
+        <v>501</v>
       </c>
       <c r="C352">
-        <v>38.093829999999997</v>
+        <v>38.061669999999999</v>
       </c>
       <c r="D352">
-        <v>-122.06973000000001</v>
+        <v>-122.01955</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -6694,13 +6700,13 @@
         <v>198</v>
       </c>
       <c r="B353">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C353">
-        <v>38.061669999999999</v>
+        <v>38.05997</v>
       </c>
       <c r="D353">
-        <v>-122.01955</v>
+        <v>-122.00397</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6708,13 +6714,13 @@
         <v>198</v>
       </c>
       <c r="B354">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C354">
-        <v>38.05997</v>
+        <v>38.059449999999998</v>
       </c>
       <c r="D354">
-        <v>-122.00397</v>
+        <v>-121.97669999999999</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6722,13 +6728,13 @@
         <v>198</v>
       </c>
       <c r="B355">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C355">
-        <v>38.059449999999998</v>
+        <v>38.04813</v>
       </c>
       <c r="D355">
-        <v>-121.97669999999999</v>
+        <v>-121.91492</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -6736,13 +6742,13 @@
         <v>198</v>
       </c>
       <c r="B356">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="C356">
-        <v>38.04813</v>
+        <v>38.059199999999997</v>
       </c>
       <c r="D356">
-        <v>-121.91492</v>
+        <v>-121.86842</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6750,13 +6756,13 @@
         <v>198</v>
       </c>
       <c r="B357">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="C357">
-        <v>38.059199999999997</v>
+        <v>38.073779999999999</v>
       </c>
       <c r="D357">
-        <v>-121.86842</v>
+        <v>-121.94725</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6764,13 +6770,13 @@
         <v>198</v>
       </c>
       <c r="B358">
-        <v>519</v>
+        <v>602</v>
       </c>
       <c r="C358">
-        <v>38.073779999999999</v>
+        <v>38.117829999999998</v>
       </c>
       <c r="D358">
-        <v>-121.94725</v>
+        <v>-122.04183</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6778,13 +6784,13 @@
         <v>198</v>
       </c>
       <c r="B359">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C359">
-        <v>38.117829999999998</v>
+        <v>38.169800000000002</v>
       </c>
       <c r="D359">
-        <v>-122.04183</v>
+        <v>-122.02177</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6792,13 +6798,13 @@
         <v>198</v>
       </c>
       <c r="B360">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C360">
-        <v>38.169800000000002</v>
+        <v>38.088700000000003</v>
       </c>
       <c r="D360">
-        <v>-122.02177</v>
+        <v>-121.88332</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6806,13 +6812,13 @@
         <v>198</v>
       </c>
       <c r="B361">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C361">
-        <v>38.088700000000003</v>
+        <v>38.16771</v>
       </c>
       <c r="D361">
-        <v>-121.88332</v>
+        <v>-121.93470000000001</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6820,13 +6826,13 @@
         <v>198</v>
       </c>
       <c r="B362">
-        <v>609</v>
+        <v>704</v>
       </c>
       <c r="C362">
-        <v>38.16771</v>
+        <v>38.070869999999999</v>
       </c>
       <c r="D362">
-        <v>-121.93470000000001</v>
+        <v>-121.77892</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6834,13 +6840,13 @@
         <v>198</v>
       </c>
       <c r="B363">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C363">
-        <v>38.070869999999999</v>
+        <v>38.090299999999999</v>
       </c>
       <c r="D363">
-        <v>-121.77892</v>
+        <v>-121.74</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -6848,13 +6854,13 @@
         <v>198</v>
       </c>
       <c r="B364">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C364">
-        <v>38.090299999999999</v>
+        <v>38.113970000000002</v>
       </c>
       <c r="D364">
-        <v>-121.74</v>
+        <v>-121.70797</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -6862,13 +6868,13 @@
         <v>198</v>
       </c>
       <c r="B365">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="C365">
-        <v>38.113970000000002</v>
+        <v>38.17595</v>
       </c>
       <c r="D365">
-        <v>-121.70797</v>
+        <v>-121.67028000000001</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -6876,13 +6882,13 @@
         <v>198</v>
       </c>
       <c r="B366">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="C366">
-        <v>38.17595</v>
+        <v>38.237870000000001</v>
       </c>
       <c r="D366">
-        <v>-121.67028000000001</v>
+        <v>-121.68438</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -6890,13 +6896,13 @@
         <v>198</v>
       </c>
       <c r="B367">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="C367">
-        <v>38.237870000000001</v>
+        <v>38.33428</v>
       </c>
       <c r="D367">
-        <v>-121.68438</v>
+        <v>-121.64733</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -6904,13 +6910,13 @@
         <v>198</v>
       </c>
       <c r="B368">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C368">
-        <v>38.33428</v>
+        <v>38.268149999999999</v>
       </c>
       <c r="D368">
-        <v>-121.64733</v>
+        <v>-121.70277</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -6918,13 +6924,13 @@
         <v>198</v>
       </c>
       <c r="B369">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C369">
-        <v>38.268149999999999</v>
+        <v>38.236150000000002</v>
       </c>
       <c r="D369">
-        <v>-121.70277</v>
+        <v>-121.67348</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -6932,13 +6938,13 @@
         <v>198</v>
       </c>
       <c r="B370">
-        <v>723</v>
+        <v>795</v>
       </c>
       <c r="C370">
-        <v>38.236150000000002</v>
+        <v>38.537700000000001</v>
       </c>
       <c r="D370">
-        <v>-121.67348</v>
+        <v>-121.58468000000001</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -6946,13 +6952,13 @@
         <v>198</v>
       </c>
       <c r="B371">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C371">
-        <v>38.537700000000001</v>
+        <v>38.473869999999998</v>
       </c>
       <c r="D371">
-        <v>-121.58468000000001</v>
+        <v>-121.5844</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -6960,13 +6966,13 @@
         <v>198</v>
       </c>
       <c r="B372">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C372">
-        <v>38.473869999999998</v>
+        <v>38.404620000000001</v>
       </c>
       <c r="D372">
-        <v>-121.5844</v>
+        <v>-121.6156</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -6974,13 +6980,13 @@
         <v>198</v>
       </c>
       <c r="B373">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="C373">
-        <v>38.404620000000001</v>
+        <v>38.03528</v>
       </c>
       <c r="D373">
-        <v>-121.6156</v>
+        <v>-121.83875</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -6988,13 +6994,13 @@
         <v>198</v>
       </c>
       <c r="B374">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C374">
-        <v>38.03528</v>
+        <v>38.02308</v>
       </c>
       <c r="D374">
-        <v>-121.83875</v>
+        <v>-121.79868</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7002,13 +7008,13 @@
         <v>198</v>
       </c>
       <c r="B375">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="C375">
-        <v>38.02308</v>
+        <v>38.051200000000001</v>
       </c>
       <c r="D375">
-        <v>-121.79868</v>
+        <v>-121.69305</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7016,13 +7022,13 @@
         <v>198</v>
       </c>
       <c r="B376">
-        <v>809</v>
+        <v>812</v>
       </c>
       <c r="C376">
-        <v>38.051200000000001</v>
+        <v>38.087919999999997</v>
       </c>
       <c r="D376">
-        <v>-121.69305</v>
+        <v>-121.64883</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7030,13 +7036,13 @@
         <v>198</v>
       </c>
       <c r="B377">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="C377">
-        <v>38.087919999999997</v>
+        <v>38.091299999999997</v>
       </c>
       <c r="D377">
-        <v>-121.64883</v>
+        <v>-121.57586999999999</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7044,13 +7050,13 @@
         <v>198</v>
       </c>
       <c r="B378">
-        <v>815</v>
+        <v>902</v>
       </c>
       <c r="C378">
-        <v>38.091299999999997</v>
+        <v>38.020499999999998</v>
       </c>
       <c r="D378">
-        <v>-121.57586999999999</v>
+        <v>-121.58255</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7058,13 +7064,13 @@
         <v>198</v>
       </c>
       <c r="B379">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="C379">
-        <v>38.020499999999998</v>
+        <v>38.054119999999998</v>
       </c>
       <c r="D379">
-        <v>-121.58255</v>
+        <v>-121.51653</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7072,13 +7078,13 @@
         <v>198</v>
       </c>
       <c r="B380">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="C380">
-        <v>38.054119999999998</v>
+        <v>38.002279999999999</v>
       </c>
       <c r="D380">
-        <v>-121.51653</v>
+        <v>-121.45037000000001</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7086,13 +7092,13 @@
         <v>198</v>
       </c>
       <c r="B381">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C381">
-        <v>38.002279999999999</v>
+        <v>37.968829999999997</v>
       </c>
       <c r="D381">
-        <v>-121.45037000000001</v>
+        <v>-121.37172</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7100,13 +7106,13 @@
         <v>198</v>
       </c>
       <c r="B382">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C382">
-        <v>37.968829999999997</v>
+        <v>37.946620000000003</v>
       </c>
       <c r="D382">
-        <v>-121.37172</v>
+        <v>-121.53475</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7114,13 +7120,13 @@
         <v>198</v>
       </c>
       <c r="B383">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C383">
-        <v>37.946620000000003</v>
+        <v>37.948999999999998</v>
       </c>
       <c r="D383">
-        <v>-121.53475</v>
+        <v>-121.55907999999999</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7128,43 +7134,43 @@
         <v>198</v>
       </c>
       <c r="B384">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="C384">
-        <v>37.948999999999998</v>
+        <v>38.105719999999998</v>
       </c>
       <c r="D384">
-        <v>-121.55907999999999</v>
+        <v>-121.49525</v>
       </c>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B385">
-        <v>919</v>
-      </c>
-      <c r="C385">
-        <v>38.105719999999998</v>
-      </c>
-      <c r="D385">
-        <v>-121.49525</v>
+      <c r="B385" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C385" s="29">
+        <v>38.0328055556</v>
+      </c>
+      <c r="D385" s="29">
+        <v>-121.869305556</v>
       </c>
     </row>
     <row r="386" spans="1:4">
       <c r="B386" s="34"/>
-      <c r="C386" s="36"/>
-      <c r="D386" s="36"/>
+      <c r="C386" s="38"/>
+      <c r="D386" s="38"/>
     </row>
     <row r="387" spans="1:4">
       <c r="B387" s="34"/>
-      <c r="C387" s="38"/>
-      <c r="D387" s="38"/>
+      <c r="C387" s="37"/>
+      <c r="D387" s="37"/>
     </row>
     <row r="388" spans="1:4">
       <c r="B388" s="34"/>
-      <c r="C388" s="37"/>
-      <c r="D388" s="37"/>
+      <c r="C388" s="36"/>
+      <c r="D388" s="36"/>
     </row>
     <row r="389" spans="1:4">
       <c r="B389" s="34"/>
@@ -7173,13 +7179,13 @@
     </row>
     <row r="390" spans="1:4">
       <c r="B390" s="34"/>
-      <c r="C390" s="36"/>
-      <c r="D390" s="36"/>
+      <c r="C390" s="37"/>
+      <c r="D390" s="35"/>
     </row>
     <row r="391" spans="1:4">
       <c r="B391" s="34"/>
       <c r="C391" s="37"/>
-      <c r="D391" s="35"/>
+      <c r="D391" s="39"/>
     </row>
     <row r="392" spans="1:4">
       <c r="B392" s="34"/>
@@ -7190,11 +7196,6 @@
       <c r="B393" s="34"/>
       <c r="C393" s="37"/>
       <c r="D393" s="39"/>
-    </row>
-    <row r="394" spans="1:4">
-      <c r="B394" s="34"/>
-      <c r="C394" s="37"/>
-      <c r="D394" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding updated EMP 2020 data and new 2020 SMSCG data, and fixed EDI links
</commit_message>
<xml_diff>
--- a/data-raw/stations.xlsx
+++ b/data-raw/stations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD00C16-6B53-4200-AAB8-BA6B45648305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7BF56D-4897-4538-B0AE-793E5ABCAA9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="402">
   <si>
     <t>Project</t>
   </si>
@@ -1857,10 +1857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G392"/>
+  <dimension ref="A1:G393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="D358" sqref="D358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6784,13 +6784,13 @@
         <v>198</v>
       </c>
       <c r="B358">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C358">
-        <v>38.169800000000002</v>
+        <v>38.148530000000001</v>
       </c>
       <c r="D358">
-        <v>-122.02177</v>
+        <v>-122.05737999999999</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6798,13 +6798,13 @@
         <v>198</v>
       </c>
       <c r="B359">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C359">
-        <v>38.088700000000003</v>
+        <v>38.169800000000002</v>
       </c>
       <c r="D359">
-        <v>-121.88332</v>
+        <v>-122.02177</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6812,13 +6812,13 @@
         <v>198</v>
       </c>
       <c r="B360">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C360">
-        <v>38.16771</v>
+        <v>38.088700000000003</v>
       </c>
       <c r="D360">
-        <v>-121.93470000000001</v>
+        <v>-121.88332</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6826,13 +6826,13 @@
         <v>198</v>
       </c>
       <c r="B361">
-        <v>704</v>
+        <v>609</v>
       </c>
       <c r="C361">
-        <v>38.070869999999999</v>
+        <v>38.16771</v>
       </c>
       <c r="D361">
-        <v>-121.77892</v>
+        <v>-121.93470000000001</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6840,13 +6840,13 @@
         <v>198</v>
       </c>
       <c r="B362">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C362">
-        <v>38.090299999999999</v>
+        <v>38.070869999999999</v>
       </c>
       <c r="D362">
-        <v>-121.74</v>
+        <v>-121.77892</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6854,13 +6854,13 @@
         <v>198</v>
       </c>
       <c r="B363">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C363">
-        <v>38.113970000000002</v>
+        <v>38.090299999999999</v>
       </c>
       <c r="D363">
-        <v>-121.70797</v>
+        <v>-121.74</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -6868,13 +6868,13 @@
         <v>198</v>
       </c>
       <c r="B364">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C364">
-        <v>38.17595</v>
+        <v>38.113970000000002</v>
       </c>
       <c r="D364">
-        <v>-121.67028000000001</v>
+        <v>-121.70797</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -6882,13 +6882,13 @@
         <v>198</v>
       </c>
       <c r="B365">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="C365">
-        <v>38.237870000000001</v>
+        <v>38.17595</v>
       </c>
       <c r="D365">
-        <v>-121.68438</v>
+        <v>-121.67028000000001</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -6896,13 +6896,13 @@
         <v>198</v>
       </c>
       <c r="B366">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C366">
-        <v>38.33428</v>
+        <v>38.237870000000001</v>
       </c>
       <c r="D366">
-        <v>-121.64733</v>
+        <v>-121.68438</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -6910,13 +6910,13 @@
         <v>198</v>
       </c>
       <c r="B367">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C367">
-        <v>38.268149999999999</v>
+        <v>38.33428</v>
       </c>
       <c r="D367">
-        <v>-121.70277</v>
+        <v>-121.64733</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -6924,13 +6924,13 @@
         <v>198</v>
       </c>
       <c r="B368">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C368">
-        <v>38.236150000000002</v>
+        <v>38.268149999999999</v>
       </c>
       <c r="D368">
-        <v>-121.67348</v>
+        <v>-121.70277</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -6938,13 +6938,13 @@
         <v>198</v>
       </c>
       <c r="B369">
-        <v>795</v>
+        <v>723</v>
       </c>
       <c r="C369">
-        <v>38.537700000000001</v>
+        <v>38.236150000000002</v>
       </c>
       <c r="D369">
-        <v>-121.58468000000001</v>
+        <v>-121.67348</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -6952,13 +6952,13 @@
         <v>198</v>
       </c>
       <c r="B370">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C370">
-        <v>38.473869999999998</v>
+        <v>38.537700000000001</v>
       </c>
       <c r="D370">
-        <v>-121.5844</v>
+        <v>-121.58468000000001</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -6966,13 +6966,13 @@
         <v>198</v>
       </c>
       <c r="B371">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C371">
-        <v>38.404620000000001</v>
+        <v>38.473869999999998</v>
       </c>
       <c r="D371">
-        <v>-121.6156</v>
+        <v>-121.5844</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -6980,13 +6980,13 @@
         <v>198</v>
       </c>
       <c r="B372">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="C372">
-        <v>38.03528</v>
+        <v>38.404620000000001</v>
       </c>
       <c r="D372">
-        <v>-121.83875</v>
+        <v>-121.6156</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -6994,13 +6994,13 @@
         <v>198</v>
       </c>
       <c r="B373">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C373">
-        <v>38.02308</v>
+        <v>38.03528</v>
       </c>
       <c r="D373">
-        <v>-121.79868</v>
+        <v>-121.83875</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7008,13 +7008,13 @@
         <v>198</v>
       </c>
       <c r="B374">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="C374">
-        <v>38.051200000000001</v>
+        <v>38.02308</v>
       </c>
       <c r="D374">
-        <v>-121.69305</v>
+        <v>-121.79868</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7022,13 +7022,13 @@
         <v>198</v>
       </c>
       <c r="B375">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C375">
-        <v>38.087919999999997</v>
+        <v>38.051200000000001</v>
       </c>
       <c r="D375">
-        <v>-121.64883</v>
+        <v>-121.69305</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7036,13 +7036,13 @@
         <v>198</v>
       </c>
       <c r="B376">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C376">
-        <v>38.091299999999997</v>
+        <v>38.087919999999997</v>
       </c>
       <c r="D376">
-        <v>-121.57586999999999</v>
+        <v>-121.64883</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7050,13 +7050,13 @@
         <v>198</v>
       </c>
       <c r="B377">
-        <v>902</v>
+        <v>815</v>
       </c>
       <c r="C377">
-        <v>38.020499999999998</v>
+        <v>38.091299999999997</v>
       </c>
       <c r="D377">
-        <v>-121.58255</v>
+        <v>-121.57586999999999</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7064,13 +7064,13 @@
         <v>198</v>
       </c>
       <c r="B378">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C378">
-        <v>38.054119999999998</v>
+        <v>38.020499999999998</v>
       </c>
       <c r="D378">
-        <v>-121.51653</v>
+        <v>-121.58255</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7078,13 +7078,13 @@
         <v>198</v>
       </c>
       <c r="B379">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C379">
-        <v>38.002279999999999</v>
+        <v>38.054119999999998</v>
       </c>
       <c r="D379">
-        <v>-121.45037000000001</v>
+        <v>-121.51653</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7092,13 +7092,13 @@
         <v>198</v>
       </c>
       <c r="B380">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C380">
-        <v>37.968829999999997</v>
+        <v>38.002279999999999</v>
       </c>
       <c r="D380">
-        <v>-121.37172</v>
+        <v>-121.45037000000001</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7106,13 +7106,13 @@
         <v>198</v>
       </c>
       <c r="B381">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C381">
-        <v>37.946620000000003</v>
+        <v>37.968829999999997</v>
       </c>
       <c r="D381">
-        <v>-121.53475</v>
+        <v>-121.37172</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7120,13 +7120,13 @@
         <v>198</v>
       </c>
       <c r="B382">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C382">
-        <v>37.948999999999998</v>
+        <v>37.946620000000003</v>
       </c>
       <c r="D382">
-        <v>-121.55907999999999</v>
+        <v>-121.53475</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7134,68 +7134,82 @@
         <v>198</v>
       </c>
       <c r="B383">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="C383">
-        <v>38.105719999999998</v>
+        <v>37.948999999999998</v>
       </c>
       <c r="D383">
-        <v>-121.49525</v>
+        <v>-121.55907999999999</v>
       </c>
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B384" s="28" t="s">
+      <c r="B384">
+        <v>919</v>
+      </c>
+      <c r="C384">
+        <v>38.105719999999998</v>
+      </c>
+      <c r="D384">
+        <v>-121.49525</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4">
+      <c r="A385" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B385" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="C384" s="29">
+      <c r="C385" s="29">
         <v>38.0328055556</v>
       </c>
-      <c r="D384" s="29">
+      <c r="D385" s="29">
         <v>-121.869305556</v>
       </c>
     </row>
-    <row r="385" spans="2:4">
-      <c r="B385" s="34"/>
-      <c r="C385" s="38"/>
-      <c r="D385" s="38"/>
-    </row>
-    <row r="386" spans="2:4">
+    <row r="386" spans="1:4">
       <c r="B386" s="34"/>
-      <c r="C386" s="37"/>
-      <c r="D386" s="37"/>
-    </row>
-    <row r="387" spans="2:4">
+      <c r="C386" s="38"/>
+      <c r="D386" s="38"/>
+    </row>
+    <row r="387" spans="1:4">
       <c r="B387" s="34"/>
-      <c r="C387" s="36"/>
-      <c r="D387" s="36"/>
-    </row>
-    <row r="388" spans="2:4">
+      <c r="C387" s="37"/>
+      <c r="D387" s="37"/>
+    </row>
+    <row r="388" spans="1:4">
       <c r="B388" s="34"/>
       <c r="C388" s="36"/>
       <c r="D388" s="36"/>
     </row>
-    <row r="389" spans="2:4">
+    <row r="389" spans="1:4">
       <c r="B389" s="34"/>
-      <c r="C389" s="37"/>
-      <c r="D389" s="35"/>
-    </row>
-    <row r="390" spans="2:4">
+      <c r="C389" s="36"/>
+      <c r="D389" s="36"/>
+    </row>
+    <row r="390" spans="1:4">
       <c r="B390" s="34"/>
       <c r="C390" s="37"/>
-      <c r="D390" s="39"/>
-    </row>
-    <row r="391" spans="2:4">
+      <c r="D390" s="35"/>
+    </row>
+    <row r="391" spans="1:4">
       <c r="B391" s="34"/>
       <c r="C391" s="37"/>
       <c r="D391" s="39"/>
     </row>
-    <row r="392" spans="2:4">
+    <row r="392" spans="1:4">
       <c r="B392" s="34"/>
       <c r="C392" s="37"/>
       <c r="D392" s="39"/>
+    </row>
+    <row r="393" spans="1:4">
+      <c r="B393" s="34"/>
+      <c r="C393" s="37"/>
+      <c r="D393" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on adding YBFMP to zooper
</commit_message>
<xml_diff>
--- a/data-raw/stations.xlsx
+++ b/data-raw/stations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7BF56D-4897-4538-B0AE-793E5ABCAA9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB67B458-BB99-4508-B6AE-1D0D3DA94694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="405">
   <si>
     <t>Project</t>
   </si>
@@ -1241,16 +1241,24 @@
   </si>
   <si>
     <t>FRP Grizz</t>
+  </si>
+  <si>
+    <t>YBFMP</t>
+  </si>
+  <si>
+    <t>SHR</t>
+  </si>
+  <si>
+    <t>STTD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1478,7 +1486,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1559,7 +1567,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1859,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="D358" sqref="D358"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="F385" sqref="F385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3693,13 +3700,13 @@
       <c r="A133" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="B133" s="40" t="s">
+      <c r="B133" s="39" t="s">
         <v>399</v>
       </c>
-      <c r="C133" s="41">
+      <c r="C133" s="40">
         <v>38.143865830000003</v>
       </c>
-      <c r="D133" s="41">
+      <c r="D133" s="40">
         <v>-121.90888889</v>
       </c>
     </row>
@@ -3707,13 +3714,13 @@
       <c r="A134" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="B134" s="40" t="s">
+      <c r="B134" s="39" t="s">
         <v>400</v>
       </c>
-      <c r="C134" s="41">
+      <c r="C134" s="40">
         <v>38.072800000000001</v>
       </c>
-      <c r="D134" s="41">
+      <c r="D134" s="40">
         <v>-121.92111111</v>
       </c>
     </row>
@@ -3721,13 +3728,13 @@
       <c r="A135" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="B135" s="40" t="s">
+      <c r="B135" s="39" t="s">
         <v>401</v>
       </c>
-      <c r="C135" s="42">
+      <c r="C135" s="41">
         <v>38.113421000000002</v>
       </c>
-      <c r="D135" s="41">
+      <c r="D135" s="40">
         <v>-121.98896999999999</v>
       </c>
     </row>
@@ -7172,14 +7179,32 @@
       </c>
     </row>
     <row r="386" spans="1:4">
-      <c r="B386" s="34"/>
-      <c r="C386" s="38"/>
-      <c r="D386" s="38"/>
+      <c r="A386" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B386" t="s">
+        <v>403</v>
+      </c>
+      <c r="C386">
+        <v>38.531880999999998</v>
+      </c>
+      <c r="D386">
+        <v>-121.527912</v>
+      </c>
     </row>
     <row r="387" spans="1:4">
-      <c r="B387" s="34"/>
-      <c r="C387" s="37"/>
-      <c r="D387" s="37"/>
+      <c r="A387" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B387" t="s">
+        <v>404</v>
+      </c>
+      <c r="C387">
+        <v>38.353383000000001</v>
+      </c>
+      <c r="D387">
+        <v>-121.643181</v>
+      </c>
     </row>
     <row r="388" spans="1:4">
       <c r="B388" s="34"/>
@@ -7199,17 +7224,17 @@
     <row r="391" spans="1:4">
       <c r="B391" s="34"/>
       <c r="C391" s="37"/>
-      <c r="D391" s="39"/>
+      <c r="D391" s="38"/>
     </row>
     <row r="392" spans="1:4">
       <c r="B392" s="34"/>
       <c r="C392" s="37"/>
-      <c r="D392" s="39"/>
+      <c r="D392" s="38"/>
     </row>
     <row r="393" spans="1:4">
       <c r="B393" s="34"/>
       <c r="C393" s="37"/>
-      <c r="D393" s="39"/>
+      <c r="D393" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added newest FMWT/STN data, including new station STN 722
</commit_message>
<xml_diff>
--- a/data-raw/stations.xlsx
+++ b/data-raw/stations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\zooper\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB67B458-BB99-4508-B6AE-1D0D3DA94694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BDC87D-4BF2-4C6C-B5A2-DEE3B82E5600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="405">
   <si>
     <t>Project</t>
   </si>
@@ -1864,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G393"/>
+  <dimension ref="A1:G394"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
-      <selection activeCell="F385" sqref="F385"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136:D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3740,10 +3740,16 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="32" t="s">
-        <v>397</v>
-      </c>
-      <c r="B136" s="33">
-        <v>997</v>
+        <v>238</v>
+      </c>
+      <c r="B136">
+        <v>722</v>
+      </c>
+      <c r="C136">
+        <v>38.255028000000003</v>
+      </c>
+      <c r="D136">
+        <v>-121.68858299999999</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3751,7 +3757,7 @@
         <v>397</v>
       </c>
       <c r="B137" s="33">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3759,7 +3765,7 @@
         <v>397</v>
       </c>
       <c r="B138" s="33">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3767,13 +3773,7 @@
         <v>397</v>
       </c>
       <c r="B139" s="33">
-        <v>323</v>
-      </c>
-      <c r="C139" s="29">
-        <v>38.042888888888889</v>
-      </c>
-      <c r="D139" s="29">
-        <v>-122.28630555555556</v>
+        <v>999</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3781,13 +3781,13 @@
         <v>397</v>
       </c>
       <c r="B140" s="33">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C140" s="29">
-        <v>38.060305555555551</v>
+        <v>38.042888888888889</v>
       </c>
       <c r="D140" s="29">
-        <v>-122.35</v>
+        <v>-122.28630555555556</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3795,13 +3795,13 @@
         <v>397</v>
       </c>
       <c r="B141" s="33">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C141" s="29">
-        <v>38.063611111111108</v>
+        <v>38.060305555555551</v>
       </c>
       <c r="D141" s="29">
-        <v>-122.304</v>
+        <v>-122.35</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3809,13 +3809,13 @@
         <v>397</v>
       </c>
       <c r="B142" s="33">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C142" s="29">
-        <v>38.076388888888893</v>
+        <v>38.063611111111108</v>
       </c>
       <c r="D142" s="29">
-        <v>-122.33799999999999</v>
+        <v>-122.304</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3823,13 +3823,13 @@
         <v>397</v>
       </c>
       <c r="B143" s="33">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C143" s="29">
-        <v>38.071111111111115</v>
+        <v>38.076388888888893</v>
       </c>
       <c r="D143" s="29">
-        <v>-122.324</v>
+        <v>-122.33799999999999</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3837,13 +3837,13 @@
         <v>397</v>
       </c>
       <c r="B144" s="33">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C144" s="29">
-        <v>38.061083333333329</v>
+        <v>38.071111111111115</v>
       </c>
       <c r="D144" s="29">
-        <v>-122.27800000000001</v>
+        <v>-122.324</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3851,13 +3851,13 @@
         <v>397</v>
       </c>
       <c r="B145" s="33">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C145" s="29">
-        <v>38.099222222222224</v>
+        <v>38.061083333333329</v>
       </c>
       <c r="D145" s="29">
-        <v>-122.26327777777777</v>
+        <v>-122.27800000000001</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3865,13 +3865,13 @@
         <v>397</v>
       </c>
       <c r="B146" s="33">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C146" s="29">
-        <v>38.127250000000004</v>
+        <v>38.099222222222224</v>
       </c>
       <c r="D146" s="29">
-        <v>-122.27877777777778</v>
+        <v>-122.26327777777777</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3879,13 +3879,13 @@
         <v>397</v>
       </c>
       <c r="B147" s="33">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C147" s="29">
-        <v>38.146250000000002</v>
+        <v>38.127250000000004</v>
       </c>
       <c r="D147" s="29">
-        <v>-122.28874999999999</v>
+        <v>-122.27877777777778</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3893,13 +3893,13 @@
         <v>397</v>
       </c>
       <c r="B148" s="33">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C148" s="29">
-        <v>38.182361111111106</v>
+        <v>38.146250000000002</v>
       </c>
       <c r="D148" s="29">
-        <v>-122.30927777777778</v>
+        <v>-122.28874999999999</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3907,13 +3907,13 @@
         <v>397</v>
       </c>
       <c r="B149" s="33">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C149" s="29">
-        <v>38.212694444444445</v>
+        <v>38.182361111111106</v>
       </c>
       <c r="D149" s="29">
-        <v>-122.30869444444444</v>
+        <v>-122.30927777777778</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3921,13 +3921,13 @@
         <v>397</v>
       </c>
       <c r="B150" s="33">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C150" s="29">
-        <v>38.223833333333339</v>
+        <v>38.212694444444445</v>
       </c>
       <c r="D150" s="29">
-        <v>-122.30897222222222</v>
+        <v>-122.30869444444444</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3935,13 +3935,13 @@
         <v>397</v>
       </c>
       <c r="B151" s="33">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C151" s="29">
-        <v>38.236388888888889</v>
+        <v>38.223833333333339</v>
       </c>
       <c r="D151" s="29">
-        <v>-122.28716666666666</v>
+        <v>-122.30897222222222</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3949,13 +3949,13 @@
         <v>397</v>
       </c>
       <c r="B152" s="33">
-        <v>405</v>
+        <v>346</v>
       </c>
       <c r="C152" s="29">
-        <v>38.039916666666663</v>
+        <v>38.236388888888889</v>
       </c>
       <c r="D152" s="29">
-        <v>-122.14672222222222</v>
+        <v>-122.28716666666666</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3963,13 +3963,13 @@
         <v>397</v>
       </c>
       <c r="B153" s="33">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C153" s="29">
-        <v>38.050222222222217</v>
+        <v>38.039916666666663</v>
       </c>
       <c r="D153" s="29">
-        <v>-122.07652777777777</v>
+        <v>-122.14672222222222</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3977,13 +3977,13 @@
         <v>397</v>
       </c>
       <c r="B154" s="33">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C154" s="29">
-        <v>38.067500000000003</v>
+        <v>38.050222222222217</v>
       </c>
       <c r="D154" s="29">
-        <v>-122.09555555555555</v>
+        <v>-122.07652777777777</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3991,13 +3991,13 @@
         <v>397</v>
       </c>
       <c r="B155" s="33">
-        <v>501</v>
+        <v>418</v>
       </c>
       <c r="C155" s="29">
-        <v>38.073333333333338</v>
+        <v>38.067500000000003</v>
       </c>
       <c r="D155" s="29">
-        <v>-122.02633333333333</v>
+        <v>-122.09555555555555</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -4005,13 +4005,13 @@
         <v>397</v>
       </c>
       <c r="B156" s="33">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C156" s="29">
-        <v>38.051944444444445</v>
+        <v>38.073333333333338</v>
       </c>
       <c r="D156" s="29">
-        <v>-121.98608333333334</v>
+        <v>-122.02633333333333</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4019,13 +4019,13 @@
         <v>397</v>
       </c>
       <c r="B157" s="33">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C157" s="29">
-        <v>38.047166666666662</v>
+        <v>38.051944444444445</v>
       </c>
       <c r="D157" s="29">
-        <v>-121.91722222222222</v>
+        <v>-121.98608333333334</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4033,13 +4033,13 @@
         <v>397</v>
       </c>
       <c r="B158" s="33">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C158" s="29">
-        <v>38.058861111111106</v>
+        <v>38.047166666666662</v>
       </c>
       <c r="D158" s="29">
-        <v>-121.86774999999999</v>
+        <v>-121.91722222222222</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4047,13 +4047,13 @@
         <v>397</v>
       </c>
       <c r="B159" s="33">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C159" s="29">
-        <v>38.074750000000002</v>
+        <v>38.058861111111106</v>
       </c>
       <c r="D159" s="29">
-        <v>-121.95808333333333</v>
+        <v>-121.86774999999999</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4061,13 +4061,13 @@
         <v>397</v>
       </c>
       <c r="B160" s="33">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C160" s="29">
-        <v>38.032166666666669</v>
+        <v>38.074750000000002</v>
       </c>
       <c r="D160" s="29">
-        <v>-121.86311111111111</v>
+        <v>-121.95808333333333</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -4075,13 +4075,13 @@
         <v>397</v>
       </c>
       <c r="B161" s="33">
-        <v>602</v>
+        <v>520</v>
       </c>
       <c r="C161" s="29">
-        <v>38.115555555555559</v>
+        <v>38.032166666666669</v>
       </c>
       <c r="D161" s="29">
-        <v>-122.04239166666666</v>
+        <v>-121.86311111111111</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -4089,13 +4089,13 @@
         <v>397</v>
       </c>
       <c r="B162" s="33">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C162" s="29">
-        <v>38.170583333333333</v>
+        <v>38.115555555555559</v>
       </c>
       <c r="D162" s="29">
-        <v>-122.02791666666667</v>
+        <v>-122.04239166666666</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -4103,13 +4103,13 @@
         <v>397</v>
       </c>
       <c r="B163" s="33">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C163" s="29">
-        <v>38.167083333333331</v>
+        <v>38.170583333333333</v>
       </c>
       <c r="D163" s="29">
-        <v>-121.93783333333333</v>
+        <v>-122.02791666666667</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -4117,13 +4117,13 @@
         <v>397</v>
       </c>
       <c r="B164" s="33">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C164" s="29">
-        <v>38.122194444444446</v>
+        <v>38.167083333333331</v>
       </c>
       <c r="D164" s="29">
-        <v>-121.88911111111112</v>
+        <v>-121.93783333333333</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -4131,13 +4131,13 @@
         <v>397</v>
       </c>
       <c r="B165" s="33">
-        <v>703</v>
+        <v>610</v>
       </c>
       <c r="C165" s="29">
-        <v>38.048611111111107</v>
+        <v>38.122194444444446</v>
       </c>
       <c r="D165" s="29">
-        <v>-121.79738888888889</v>
+        <v>-121.88911111111112</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -4145,43 +4145,43 @@
         <v>397</v>
       </c>
       <c r="B166" s="33">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C166" s="29">
-        <v>38.066583333333334</v>
+        <v>38.048611111111107</v>
       </c>
       <c r="D166" s="29">
-        <v>-121.79031111111111</v>
-      </c>
-      <c r="F166" s="24"/>
-      <c r="G166" s="24"/>
+        <v>-121.79738888888889</v>
+      </c>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="32" t="s">
         <v>397</v>
       </c>
       <c r="B167" s="33">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C167" s="29">
-        <v>38.097611111111114</v>
+        <v>38.066583333333334</v>
       </c>
       <c r="D167" s="29">
-        <v>-121.70875000000001</v>
-      </c>
+        <v>-121.79031111111111</v>
+      </c>
+      <c r="F167" s="24"/>
+      <c r="G167" s="24"/>
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="32" t="s">
         <v>397</v>
       </c>
       <c r="B168" s="33">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C168" s="29">
-        <v>38.086083333333335</v>
+        <v>38.097611111111114</v>
       </c>
       <c r="D168" s="29">
-        <v>-121.75044444444444</v>
+        <v>-121.70875000000001</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4189,13 +4189,13 @@
         <v>397</v>
       </c>
       <c r="B169" s="33">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C169" s="29">
-        <v>38.114694444444446</v>
+        <v>38.086083333333335</v>
       </c>
       <c r="D169" s="29">
-        <v>-121.70786111111111</v>
+        <v>-121.75044444444444</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4203,13 +4203,13 @@
         <v>397</v>
       </c>
       <c r="B170" s="33">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C170" s="29">
-        <v>38.177416666666666</v>
+        <v>38.114694444444446</v>
       </c>
       <c r="D170" s="29">
-        <v>-121.66225</v>
+        <v>-121.70786111111111</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4217,13 +4217,13 @@
         <v>397</v>
       </c>
       <c r="B171" s="33">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="C171" s="29">
-        <v>38.238555555555557</v>
+        <v>38.177416666666666</v>
       </c>
       <c r="D171" s="29">
-        <v>-121.68391666666668</v>
+        <v>-121.66225</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4231,13 +4231,13 @@
         <v>397</v>
       </c>
       <c r="B172" s="33">
-        <v>801</v>
+        <v>716</v>
       </c>
       <c r="C172" s="29">
-        <v>38.043694444444441</v>
+        <v>38.238555555555557</v>
       </c>
       <c r="D172" s="29">
-        <v>-121.84399999999999</v>
+        <v>-121.68391666666668</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4245,13 +4245,13 @@
         <v>397</v>
       </c>
       <c r="B173" s="33">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C173" s="29">
-        <v>38.020833333333336</v>
+        <v>38.043694444444441</v>
       </c>
       <c r="D173" s="29">
-        <v>-121.7303888888889</v>
+        <v>-121.84399999999999</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4259,13 +4259,13 @@
         <v>397</v>
       </c>
       <c r="B174" s="33">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C174" s="29">
-        <v>38.016444444444446</v>
+        <v>38.020833333333336</v>
       </c>
       <c r="D174" s="29">
-        <v>-121.79130555555555</v>
+        <v>-121.7303888888889</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4273,13 +4273,13 @@
         <v>397</v>
       </c>
       <c r="B175" s="33">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="C175" s="29">
-        <v>38.053777777777775</v>
+        <v>38.016444444444446</v>
       </c>
       <c r="D175" s="29">
-        <v>-121.69302777777779</v>
+        <v>-121.79130555555555</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4287,13 +4287,13 @@
         <v>397</v>
       </c>
       <c r="B176" s="33">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C176" s="29">
-        <v>38.089916666666667</v>
+        <v>38.053777777777775</v>
       </c>
       <c r="D176" s="29">
-        <v>-121.63991666666668</v>
+        <v>-121.69302777777779</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4301,13 +4301,13 @@
         <v>397</v>
       </c>
       <c r="B177" s="33">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C177" s="29">
-        <v>38.087138888888894</v>
+        <v>38.089916666666667</v>
       </c>
       <c r="D177" s="29">
-        <v>-121.57113888888888</v>
+        <v>-121.63991666666668</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4315,13 +4315,13 @@
         <v>397</v>
       </c>
       <c r="B178" s="33">
-        <v>901</v>
+        <v>815</v>
       </c>
       <c r="C178" s="29">
-        <v>38.046250000000001</v>
+        <v>38.087138888888894</v>
       </c>
       <c r="D178" s="29">
-        <v>-121.6185</v>
+        <v>-121.57113888888888</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4329,13 +4329,13 @@
         <v>397</v>
       </c>
       <c r="B179" s="33">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C179" s="29">
-        <v>38.020388888888888</v>
+        <v>38.046250000000001</v>
       </c>
       <c r="D179" s="29">
-        <v>-121.58266666666667</v>
+        <v>-121.6185</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4343,13 +4343,13 @@
         <v>397</v>
       </c>
       <c r="B180" s="33">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C180" s="29">
-        <v>38.050027777777778</v>
+        <v>38.020388888888888</v>
       </c>
       <c r="D180" s="29">
-        <v>-121.50647222222223</v>
+        <v>-121.58266666666667</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4357,13 +4357,13 @@
         <v>397</v>
       </c>
       <c r="B181" s="33">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C181" s="29">
-        <v>38.005000000000003</v>
+        <v>38.050027777777778</v>
       </c>
       <c r="D181" s="29">
-        <v>-121.45302777777778</v>
+        <v>-121.50647222222223</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4371,13 +4371,13 @@
         <v>397</v>
       </c>
       <c r="B182" s="33">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C182" s="29">
-        <v>37.966416666666667</v>
+        <v>38.005000000000003</v>
       </c>
       <c r="D182" s="29">
-        <v>-121.36855555555555</v>
+        <v>-121.45302777777778</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4385,13 +4385,13 @@
         <v>397</v>
       </c>
       <c r="B183" s="33">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C183" s="29">
-        <v>37.971499999999999</v>
+        <v>37.966416666666667</v>
       </c>
       <c r="D183" s="29">
-        <v>-121.52</v>
+        <v>-121.36855555555555</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4399,13 +4399,13 @@
         <v>397</v>
       </c>
       <c r="B184" s="33">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C184" s="29">
-        <v>37.944277777777778</v>
+        <v>37.971499999999999</v>
       </c>
       <c r="D184" s="29">
-        <v>-121.56788888888889</v>
+        <v>-121.52</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4413,13 +4413,13 @@
         <v>397</v>
       </c>
       <c r="B185" s="33">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C185" s="29">
-        <v>37.859000000000002</v>
+        <v>37.944277777777778</v>
       </c>
       <c r="D185" s="29">
-        <v>-121.56713888888889</v>
+        <v>-121.56788888888889</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4427,13 +4427,13 @@
         <v>397</v>
       </c>
       <c r="B186" s="33">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C186" s="29">
-        <v>38.105194444444443</v>
+        <v>37.859000000000002</v>
       </c>
       <c r="D186" s="29">
-        <v>-121.49458333333334</v>
+        <v>-121.56713888888889</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4441,13 +4441,13 @@
         <v>397</v>
       </c>
       <c r="B187" s="33">
-        <v>330</v>
+        <v>919</v>
       </c>
       <c r="C187" s="29">
-        <v>38.063611111111108</v>
+        <v>38.105194444444443</v>
       </c>
       <c r="D187" s="29">
-        <v>-122.304</v>
+        <v>-121.49458333333334</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4455,13 +4455,13 @@
         <v>397</v>
       </c>
       <c r="B188" s="33">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="C188" s="29">
-        <v>38.253611111111113</v>
+        <v>38.063611111111108</v>
       </c>
       <c r="D188" s="29">
-        <v>-122.28469444444444</v>
+        <v>-122.304</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4469,13 +4469,13 @@
         <v>397</v>
       </c>
       <c r="B189" s="33">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C189" s="29">
-        <v>38.274361111111112</v>
+        <v>38.253611111111113</v>
       </c>
       <c r="D189" s="29">
-        <v>-122.28352777777778</v>
+        <v>-122.28469444444444</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4483,13 +4483,13 @@
         <v>397</v>
       </c>
       <c r="B190" s="33">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C190" s="29">
-        <v>38.286333333333332</v>
+        <v>38.274361111111112</v>
       </c>
       <c r="D190" s="29">
-        <v>-122.28436111111111</v>
+        <v>-122.28352777777778</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4497,13 +4497,13 @@
         <v>397</v>
       </c>
       <c r="B191" s="33">
-        <v>718</v>
+        <v>349</v>
       </c>
       <c r="C191" s="29">
-        <v>38.257555555555555</v>
+        <v>38.286333333333332</v>
       </c>
       <c r="D191" s="29">
-        <v>-121.72902777777777</v>
+        <v>-122.28436111111111</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4511,13 +4511,13 @@
         <v>397</v>
       </c>
       <c r="B192" s="33">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C192" s="29">
-        <v>38.262638888888887</v>
+        <v>38.257555555555555</v>
       </c>
       <c r="D192" s="29">
-        <v>-121.77927777777778</v>
+        <v>-121.72902777777777</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4525,13 +4525,13 @@
         <v>397</v>
       </c>
       <c r="B193" s="33">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C193" s="29">
-        <v>38.237250000000003</v>
+        <v>38.262638888888887</v>
       </c>
       <c r="D193" s="29">
-        <v>-121.67308333333334</v>
+        <v>-121.77927777777778</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4539,13 +4539,13 @@
         <v>397</v>
       </c>
       <c r="B194" s="33">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C194" s="29">
-        <v>38.256250000000001</v>
+        <v>38.237250000000003</v>
       </c>
       <c r="D194" s="29">
-        <v>-121.65208333333334</v>
+        <v>-121.67308333333334</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4553,7 +4553,13 @@
         <v>397</v>
       </c>
       <c r="B195" s="33">
-        <v>794</v>
+        <v>724</v>
+      </c>
+      <c r="C195" s="29">
+        <v>38.256250000000001</v>
+      </c>
+      <c r="D195" s="29">
+        <v>-121.65208333333334</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4561,7 +4567,7 @@
         <v>397</v>
       </c>
       <c r="B196" s="33">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4569,7 +4575,7 @@
         <v>397</v>
       </c>
       <c r="B197" s="33">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4577,7 +4583,7 @@
         <v>397</v>
       </c>
       <c r="B198" s="33">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4585,7 +4591,7 @@
         <v>397</v>
       </c>
       <c r="B199" s="33">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4593,7 +4599,7 @@
         <v>397</v>
       </c>
       <c r="B200" s="33">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4601,13 +4607,7 @@
         <v>397</v>
       </c>
       <c r="B201" s="33">
-        <v>726</v>
-      </c>
-      <c r="C201" s="29">
-        <v>38.283055555555556</v>
-      </c>
-      <c r="D201" s="29">
-        <v>-121.64383333333333</v>
+        <v>799</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4615,27 +4615,27 @@
         <v>397</v>
       </c>
       <c r="B202" s="33">
+        <v>726</v>
+      </c>
+      <c r="C202" s="29">
+        <v>38.283055555555556</v>
+      </c>
+      <c r="D202" s="29">
+        <v>-121.64383333333333</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="B203" s="33">
         <v>719</v>
       </c>
-      <c r="C202" s="29">
+      <c r="C203" s="29">
         <v>38.333500000000001</v>
       </c>
-      <c r="D202" s="29">
+      <c r="D203" s="29">
         <v>-121.64750000000001</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="28" t="s">
-        <v>391</v>
-      </c>
-      <c r="B203" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="C203" s="30">
-        <v>38.074469999999998</v>
-      </c>
-      <c r="D203" s="30">
-        <v>-122.01588</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4643,13 +4643,13 @@
         <v>391</v>
       </c>
       <c r="B204" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C204" s="30">
-        <v>38.044820000000001</v>
+        <v>38.074469999999998</v>
       </c>
       <c r="D204" s="30">
-        <v>-121.87193000000001</v>
+        <v>-122.01588</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4657,13 +4657,13 @@
         <v>391</v>
       </c>
       <c r="B205" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C205" s="30">
-        <v>38.121292169999997</v>
+        <v>38.044820000000001</v>
       </c>
       <c r="D205" s="30">
-        <v>-122.0067224</v>
+        <v>-121.87193000000001</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4671,13 +4671,13 @@
         <v>391</v>
       </c>
       <c r="B206" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C206" s="30">
-        <v>38.181780430000003</v>
+        <v>38.121292169999997</v>
       </c>
       <c r="D206" s="30">
-        <v>-121.91393739999999</v>
+        <v>-122.0067224</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4685,13 +4685,13 @@
         <v>391</v>
       </c>
       <c r="B207" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C207" s="30">
-        <v>38.043095299999997</v>
+        <v>38.181780430000003</v>
       </c>
       <c r="D207" s="30">
-        <v>-121.7992028</v>
+        <v>-121.91393739999999</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4699,13 +4699,13 @@
         <v>391</v>
       </c>
       <c r="B208" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C208" s="30">
-        <v>38.08988506</v>
+        <v>38.043095299999997</v>
       </c>
       <c r="D208" s="30">
-        <v>-121.7090585</v>
+        <v>-121.7992028</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4713,13 +4713,13 @@
         <v>391</v>
       </c>
       <c r="B209" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C209" s="30">
-        <v>38.082940000000001</v>
+        <v>38.08988506</v>
       </c>
       <c r="D209" s="30">
-        <v>-121.72507</v>
+        <v>-121.7090585</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4727,13 +4727,13 @@
         <v>391</v>
       </c>
       <c r="B210" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C210" s="30">
-        <v>38.259950000000003</v>
+        <v>38.082940000000001</v>
       </c>
       <c r="D210" s="30">
-        <v>-121.79259999999999</v>
+        <v>-121.72507</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4741,13 +4741,13 @@
         <v>391</v>
       </c>
       <c r="B211" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C211" s="30">
-        <v>38.243549999999999</v>
+        <v>38.259950000000003</v>
       </c>
       <c r="D211" s="30">
-        <v>-121.68453</v>
+        <v>-121.79259999999999</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4755,13 +4755,13 @@
         <v>391</v>
       </c>
       <c r="B212" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C212" s="30">
-        <v>38.242464470000002</v>
+        <v>38.243549999999999</v>
       </c>
       <c r="D212" s="30">
-        <v>-121.6618801</v>
+        <v>-121.68453</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4769,13 +4769,13 @@
         <v>391</v>
       </c>
       <c r="B213" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C213" s="30">
-        <v>38.258112920000002</v>
+        <v>38.242464470000002</v>
       </c>
       <c r="D213" s="30">
-        <v>-121.653526</v>
+        <v>-121.6618801</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4783,13 +4783,13 @@
         <v>391</v>
       </c>
       <c r="B214" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C214" s="30">
-        <v>38.042189569999998</v>
+        <v>38.258112920000002</v>
       </c>
       <c r="D214" s="30">
-        <v>-121.84445169999999</v>
+        <v>-121.653526</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4797,13 +4797,13 @@
         <v>391</v>
       </c>
       <c r="B215" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C215" s="30">
-        <v>38.265309999999999</v>
+        <v>38.042189569999998</v>
       </c>
       <c r="D215" s="30">
-        <v>-121.78379</v>
+        <v>-121.84445169999999</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4811,13 +4811,13 @@
         <v>391</v>
       </c>
       <c r="B216" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C216" s="30">
-        <v>38.267819490000001</v>
+        <v>38.265309999999999</v>
       </c>
       <c r="D216" s="30">
-        <v>-121.7898314</v>
+        <v>-121.78379</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4825,13 +4825,13 @@
         <v>391</v>
       </c>
       <c r="B217" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C217" s="30">
-        <v>38.263213780000001</v>
+        <v>38.267819490000001</v>
       </c>
       <c r="D217" s="30">
-        <v>-121.7803662</v>
+        <v>-121.7898314</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4839,13 +4839,13 @@
         <v>391</v>
       </c>
       <c r="B218" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C218" s="30">
-        <v>38.180309999999999</v>
+        <v>38.263213780000001</v>
       </c>
       <c r="D218" s="30">
-        <v>-121.90877999999999</v>
+        <v>-121.7803662</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4853,13 +4853,13 @@
         <v>391</v>
       </c>
       <c r="B219" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C219" s="30">
-        <v>38.182479999999998</v>
+        <v>38.180309999999999</v>
       </c>
       <c r="D219" s="30">
-        <v>-121.92171999999999</v>
+        <v>-121.90877999999999</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4867,13 +4867,13 @@
         <v>391</v>
       </c>
       <c r="B220" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C220" s="30">
-        <v>38.039000000000001</v>
+        <v>38.182479999999998</v>
       </c>
       <c r="D220" s="30">
-        <v>-121.85760999999999</v>
+        <v>-121.92171999999999</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4881,13 +4881,13 @@
         <v>391</v>
       </c>
       <c r="B221" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C221" s="30">
-        <v>38.040502709999998</v>
+        <v>38.039000000000001</v>
       </c>
       <c r="D221" s="30">
-        <v>-121.8675863</v>
+        <v>-121.85760999999999</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -4895,13 +4895,13 @@
         <v>391</v>
       </c>
       <c r="B222" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C222" s="30">
-        <v>38.038130160000001</v>
+        <v>38.040502709999998</v>
       </c>
       <c r="D222" s="30">
-        <v>-121.8577899</v>
+        <v>-121.8675863</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -4909,13 +4909,13 @@
         <v>391</v>
       </c>
       <c r="B223" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C223" s="30">
-        <v>38.286009999999997</v>
+        <v>38.038130160000001</v>
       </c>
       <c r="D223" s="30">
-        <v>-121.72101000000001</v>
+        <v>-121.8577899</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -4923,37 +4923,37 @@
         <v>391</v>
       </c>
       <c r="B224" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C224" s="30"/>
-      <c r="D224" s="30"/>
+        <v>271</v>
+      </c>
+      <c r="C224" s="30">
+        <v>38.286009999999997</v>
+      </c>
+      <c r="D224" s="30">
+        <v>-121.72101000000001</v>
+      </c>
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B225" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="C225" s="30">
-        <v>38.26030111</v>
-      </c>
-      <c r="D225" s="30">
-        <v>-121.7811813</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="C225" s="30"/>
+      <c r="D225" s="30"/>
     </row>
     <row r="226" spans="1:4">
       <c r="A226" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B226" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C226" s="30">
-        <v>38.259959870000003</v>
+        <v>38.26030111</v>
       </c>
       <c r="D226" s="30">
-        <v>-121.7906483</v>
+        <v>-121.7811813</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -4961,13 +4961,13 @@
         <v>391</v>
       </c>
       <c r="B227" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C227" s="30">
-        <v>38.083607880000002</v>
+        <v>38.259959870000003</v>
       </c>
       <c r="D227" s="30">
-        <v>-121.723387</v>
+        <v>-121.7906483</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -4975,13 +4975,13 @@
         <v>391</v>
       </c>
       <c r="B228" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C228" s="30">
-        <v>38.10404278</v>
+        <v>38.083607880000002</v>
       </c>
       <c r="D228" s="30">
-        <v>-121.710669</v>
+        <v>-121.723387</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -4989,13 +4989,13 @@
         <v>391</v>
       </c>
       <c r="B229" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C229" s="30">
-        <v>38.09872661</v>
+        <v>38.10404278</v>
       </c>
       <c r="D229" s="30">
-        <v>-121.7090939</v>
+        <v>-121.710669</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5003,13 +5003,13 @@
         <v>391</v>
       </c>
       <c r="B230" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C230" s="30">
-        <v>38.096895789999998</v>
+        <v>38.09872661</v>
       </c>
       <c r="D230" s="30">
-        <v>-121.7092772</v>
+        <v>-121.7090939</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5017,13 +5017,13 @@
         <v>391</v>
       </c>
       <c r="B231" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C231" s="30">
-        <v>38.085120000000003</v>
+        <v>38.096895789999998</v>
       </c>
       <c r="D231" s="30">
-        <v>-121.72336</v>
+        <v>-121.7092772</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5031,13 +5031,13 @@
         <v>391</v>
       </c>
       <c r="B232" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C232" s="30">
-        <v>38.023244210000001</v>
+        <v>38.085120000000003</v>
       </c>
       <c r="D232" s="30">
-        <v>-121.8333619</v>
+        <v>-121.72336</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5045,13 +5045,13 @@
         <v>391</v>
       </c>
       <c r="B233" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C233" s="30">
-        <v>38.021912989999997</v>
+        <v>38.023244210000001</v>
       </c>
       <c r="D233" s="30">
-        <v>-121.82532620000001</v>
+        <v>-121.8333619</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5059,13 +5059,13 @@
         <v>391</v>
       </c>
       <c r="B234" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C234" s="30">
-        <v>38.022789410000001</v>
+        <v>38.021912989999997</v>
       </c>
       <c r="D234" s="30">
-        <v>-121.8294301</v>
+        <v>-121.82532620000001</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5073,13 +5073,13 @@
         <v>391</v>
       </c>
       <c r="B235" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C235" s="30">
-        <v>38.021887560000003</v>
+        <v>38.022789410000001</v>
       </c>
       <c r="D235" s="30">
-        <v>-121.83369709999999</v>
+        <v>-121.8294301</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5087,13 +5087,13 @@
         <v>391</v>
       </c>
       <c r="B236" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C236" s="30">
-        <v>38.023757349999997</v>
+        <v>38.021887560000003</v>
       </c>
       <c r="D236" s="30">
-        <v>-121.8272565</v>
+        <v>-121.83369709999999</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5101,13 +5101,13 @@
         <v>391</v>
       </c>
       <c r="B237" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C237" s="30">
-        <v>38.024821000000003</v>
+        <v>38.023757349999997</v>
       </c>
       <c r="D237" s="30">
-        <v>-121.82608999999999</v>
+        <v>-121.8272565</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5115,13 +5115,13 @@
         <v>391</v>
       </c>
       <c r="B238" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C238" s="30">
-        <v>38.295859999999998</v>
+        <v>38.024821000000003</v>
       </c>
       <c r="D238" s="30">
-        <v>-121.68886000000001</v>
+        <v>-121.82608999999999</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5129,13 +5129,13 @@
         <v>391</v>
       </c>
       <c r="B239" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C239" s="30">
-        <v>38.296002000000001</v>
+        <v>38.295859999999998</v>
       </c>
       <c r="D239" s="30">
-        <v>-121.68651800000001</v>
+        <v>-121.68886000000001</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5143,13 +5143,13 @@
         <v>391</v>
       </c>
       <c r="B240" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C240" s="30">
-        <v>38.364139999999999</v>
+        <v>38.296002000000001</v>
       </c>
       <c r="D240" s="30">
-        <v>-121.6444767</v>
+        <v>-121.68651800000001</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5157,13 +5157,13 @@
         <v>391</v>
       </c>
       <c r="B241" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C241" s="30">
-        <v>38.03228</v>
+        <v>38.364139999999999</v>
       </c>
       <c r="D241" s="30">
-        <v>-121.47833</v>
+        <v>-121.6444767</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5171,13 +5171,13 @@
         <v>391</v>
       </c>
       <c r="B242" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C242" s="30">
-        <v>38.082587820000001</v>
+        <v>38.03228</v>
       </c>
       <c r="D242" s="30">
-        <v>-121.72807760000001</v>
+        <v>-121.47833</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5185,13 +5185,13 @@
         <v>391</v>
       </c>
       <c r="B243" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C243" s="30">
-        <v>38.084034219999999</v>
+        <v>38.082587820000001</v>
       </c>
       <c r="D243" s="30">
-        <v>-121.7146892</v>
+        <v>-121.72807760000001</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5199,13 +5199,13 @@
         <v>391</v>
       </c>
       <c r="B244" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C244" s="30">
-        <v>38.099297280000002</v>
+        <v>38.084034219999999</v>
       </c>
       <c r="D244" s="30">
-        <v>-121.7079337</v>
+        <v>-121.7146892</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5213,13 +5213,13 @@
         <v>391</v>
       </c>
       <c r="B245" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C245" s="30">
-        <v>38.303673269999997</v>
+        <v>38.099297280000002</v>
       </c>
       <c r="D245" s="30">
-        <v>-121.7312177</v>
+        <v>-121.7079337</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5227,13 +5227,13 @@
         <v>391</v>
       </c>
       <c r="B246" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C246" s="30">
-        <v>38.277729919999999</v>
+        <v>38.303673269999997</v>
       </c>
       <c r="D246" s="30">
-        <v>-121.71053860000001</v>
+        <v>-121.7312177</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5241,13 +5241,13 @@
         <v>391</v>
       </c>
       <c r="B247" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C247" s="30">
-        <v>38.242040000000003</v>
+        <v>38.277729919999999</v>
       </c>
       <c r="D247" s="30">
-        <v>-121.68239</v>
+        <v>-121.71053860000001</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5255,13 +5255,13 @@
         <v>391</v>
       </c>
       <c r="B248" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C248" s="30">
-        <v>38.277189999999997</v>
+        <v>38.242040000000003</v>
       </c>
       <c r="D248" s="30">
-        <v>-121.69405999999999</v>
+        <v>-121.68239</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5269,13 +5269,13 @@
         <v>391</v>
       </c>
       <c r="B249" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C249" s="30">
-        <v>38.246361999999998</v>
+        <v>38.277189999999997</v>
       </c>
       <c r="D249" s="30">
-        <v>-121.678139</v>
+        <v>-121.69405999999999</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5283,13 +5283,13 @@
         <v>391</v>
       </c>
       <c r="B250" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C250" s="30">
-        <v>38.269292</v>
+        <v>38.246361999999998</v>
       </c>
       <c r="D250" s="30">
-        <v>-121.691395</v>
+        <v>-121.678139</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5297,13 +5297,13 @@
         <v>391</v>
       </c>
       <c r="B251" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C251" s="30">
-        <v>38.255043000000001</v>
+        <v>38.269292</v>
       </c>
       <c r="D251" s="30">
-        <v>-121.672072</v>
+        <v>-121.691395</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5311,13 +5311,13 @@
         <v>391</v>
       </c>
       <c r="B252" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C252" s="30">
-        <v>38.257888000000001</v>
+        <v>38.255043000000001</v>
       </c>
       <c r="D252" s="30">
-        <v>-121.690273</v>
+        <v>-121.672072</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5325,13 +5325,13 @@
         <v>391</v>
       </c>
       <c r="B253" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C253" s="30">
-        <v>38.265140000000002</v>
+        <v>38.257888000000001</v>
       </c>
       <c r="D253" s="30">
-        <v>-121.67155700000001</v>
+        <v>-121.690273</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5339,13 +5339,13 @@
         <v>391</v>
       </c>
       <c r="B254" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C254" s="30">
-        <v>38.252679999999998</v>
+        <v>38.265140000000002</v>
       </c>
       <c r="D254" s="30">
-        <v>-121.686263</v>
+        <v>-121.67155700000001</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5353,13 +5353,13 @@
         <v>391</v>
       </c>
       <c r="B255" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C255" s="30">
-        <v>38.273775000000001</v>
+        <v>38.252679999999998</v>
       </c>
       <c r="D255" s="30">
-        <v>-121.66692999999999</v>
+        <v>-121.686263</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5367,13 +5367,13 @@
         <v>391</v>
       </c>
       <c r="B256" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C256" s="30">
-        <v>38.244607000000002</v>
+        <v>38.273775000000001</v>
       </c>
       <c r="D256" s="30">
-        <v>-121.686421</v>
+        <v>-121.66692999999999</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5381,13 +5381,13 @@
         <v>391</v>
       </c>
       <c r="B257" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C257" s="30">
-        <v>38.282319999999999</v>
+        <v>38.244607000000002</v>
       </c>
       <c r="D257" s="30">
-        <v>-121.69229</v>
+        <v>-121.686421</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5395,13 +5395,13 @@
         <v>391</v>
       </c>
       <c r="B258" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C258" s="30">
-        <v>38.284170000000003</v>
+        <v>38.282319999999999</v>
       </c>
       <c r="D258" s="30">
-        <v>-121.66531999999999</v>
+        <v>-121.69229</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5409,13 +5409,13 @@
         <v>391</v>
       </c>
       <c r="B259" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C259" s="30">
-        <v>38.288989999999998</v>
+        <v>38.284170000000003</v>
       </c>
       <c r="D259" s="30">
-        <v>-121.66651</v>
+        <v>-121.66531999999999</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5423,13 +5423,13 @@
         <v>391</v>
       </c>
       <c r="B260" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C260" s="30">
-        <v>38.287590000000002</v>
+        <v>38.288989999999998</v>
       </c>
       <c r="D260" s="30">
-        <v>-121.69197</v>
+        <v>-121.66651</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5437,13 +5437,13 @@
         <v>391</v>
       </c>
       <c r="B261" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C261" s="30">
-        <v>38.29607</v>
+        <v>38.287590000000002</v>
       </c>
       <c r="D261" s="30">
-        <v>-121.69193</v>
+        <v>-121.69197</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -5451,13 +5451,13 @@
         <v>391</v>
       </c>
       <c r="B262" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C262" s="30">
-        <v>38.278500000000001</v>
+        <v>38.29607</v>
       </c>
       <c r="D262" s="30">
-        <v>-121.69401999999999</v>
+        <v>-121.69193</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5465,13 +5465,13 @@
         <v>391</v>
       </c>
       <c r="B263" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C263" s="30">
-        <v>38.290030000000002</v>
+        <v>38.278500000000001</v>
       </c>
       <c r="D263" s="30">
-        <v>-121.6918</v>
+        <v>-121.69401999999999</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5479,13 +5479,13 @@
         <v>391</v>
       </c>
       <c r="B264" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C264" s="30">
-        <v>38.296169999999996</v>
+        <v>38.290030000000002</v>
       </c>
       <c r="D264" s="30">
-        <v>-121.68986</v>
+        <v>-121.6918</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5493,13 +5493,13 @@
         <v>391</v>
       </c>
       <c r="B265" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C265" s="30">
-        <v>38.269620000000003</v>
+        <v>38.296169999999996</v>
       </c>
       <c r="D265" s="30">
-        <v>-121.67718000000001</v>
+        <v>-121.68986</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5507,13 +5507,13 @@
         <v>391</v>
       </c>
       <c r="B266" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C266" s="30">
-        <v>38.275649999999999</v>
+        <v>38.269620000000003</v>
       </c>
       <c r="D266" s="30">
-        <v>-121.67599</v>
+        <v>-121.67718000000001</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5521,13 +5521,13 @@
         <v>391</v>
       </c>
       <c r="B267" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C267" s="30">
-        <v>38.249670000000002</v>
+        <v>38.275649999999999</v>
       </c>
       <c r="D267" s="30">
-        <v>-121.67701</v>
+        <v>-121.67599</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -5535,13 +5535,13 @@
         <v>391</v>
       </c>
       <c r="B268" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C268" s="30">
-        <v>38.247709999999998</v>
+        <v>38.249670000000002</v>
       </c>
       <c r="D268" s="30">
-        <v>-121.67861000000001</v>
+        <v>-121.67701</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5549,13 +5549,13 @@
         <v>391</v>
       </c>
       <c r="B269" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C269" s="30">
-        <v>38.26238</v>
+        <v>38.247709999999998</v>
       </c>
       <c r="D269" s="30">
-        <v>-121.67883</v>
+        <v>-121.67861000000001</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5563,13 +5563,13 @@
         <v>391</v>
       </c>
       <c r="B270" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C270" s="30">
-        <v>38.267040000000001</v>
+        <v>38.26238</v>
       </c>
       <c r="D270" s="30">
-        <v>-121.6879</v>
+        <v>-121.67883</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5577,13 +5577,13 @@
         <v>391</v>
       </c>
       <c r="B271" s="30" t="s">
-        <v>396</v>
+        <v>318</v>
       </c>
       <c r="C271" s="30">
-        <v>38.258663110000001</v>
+        <v>38.267040000000001</v>
       </c>
       <c r="D271" s="30">
-        <v>-121.79256650000001</v>
+        <v>-121.6879</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5591,13 +5591,13 @@
         <v>391</v>
       </c>
       <c r="B272" s="30" t="s">
-        <v>319</v>
+        <v>396</v>
       </c>
       <c r="C272" s="30">
-        <v>38.259518229999998</v>
+        <v>38.258663110000001</v>
       </c>
       <c r="D272" s="30">
-        <v>-121.79754749999999</v>
+        <v>-121.79256650000001</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5605,13 +5605,13 @@
         <v>391</v>
       </c>
       <c r="B273" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C273" s="30">
-        <v>38.259779999999999</v>
+        <v>38.259518229999998</v>
       </c>
       <c r="D273" s="30">
-        <v>-121.7923</v>
+        <v>-121.79754749999999</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5619,13 +5619,13 @@
         <v>391</v>
       </c>
       <c r="B274" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C274" s="30">
-        <v>38.25902</v>
+        <v>38.259779999999999</v>
       </c>
       <c r="D274" s="30">
-        <v>-121.79259</v>
+        <v>-121.7923</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5633,13 +5633,13 @@
         <v>391</v>
       </c>
       <c r="B275" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C275" s="30">
-        <v>38.260269030000003</v>
+        <v>38.25902</v>
       </c>
       <c r="D275" s="30">
-        <v>-121.7616752</v>
+        <v>-121.79259</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5647,13 +5647,13 @@
         <v>391</v>
       </c>
       <c r="B276" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C276" s="30">
-        <v>38.258149009999997</v>
+        <v>38.260269030000003</v>
       </c>
       <c r="D276" s="30">
-        <v>-121.73812100000001</v>
+        <v>-121.7616752</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5661,13 +5661,13 @@
         <v>391</v>
       </c>
       <c r="B277" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C277" s="30">
-        <v>38.249980829999998</v>
+        <v>38.258149009999997</v>
       </c>
       <c r="D277" s="30">
-        <v>-121.713593</v>
+        <v>-121.73812100000001</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -5675,13 +5675,13 @@
         <v>391</v>
       </c>
       <c r="B278" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C278" s="30">
-        <v>38.242319999999999</v>
+        <v>38.249980829999998</v>
       </c>
       <c r="D278" s="30">
-        <v>-121.66168</v>
+        <v>-121.713593</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5689,13 +5689,13 @@
         <v>391</v>
       </c>
       <c r="B279" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C279" s="30">
-        <v>38.256869999999999</v>
+        <v>38.242319999999999</v>
       </c>
       <c r="D279" s="30">
-        <v>-121.6527</v>
+        <v>-121.66168</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5703,13 +5703,13 @@
         <v>391</v>
       </c>
       <c r="B280" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C280" s="30">
-        <v>38.234140869999997</v>
+        <v>38.256869999999999</v>
       </c>
       <c r="D280" s="30">
-        <v>-121.6691908</v>
+        <v>-121.6527</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5717,13 +5717,13 @@
         <v>391</v>
       </c>
       <c r="B281" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C281" s="30">
-        <v>38.24640849</v>
+        <v>38.234140869999997</v>
       </c>
       <c r="D281" s="30">
-        <v>-121.6595325</v>
+        <v>-121.6691908</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5731,13 +5731,13 @@
         <v>391</v>
       </c>
       <c r="B282" s="30" t="s">
-        <v>394</v>
+        <v>328</v>
       </c>
       <c r="C282" s="30">
-        <v>38.263632440000002</v>
+        <v>38.24640849</v>
       </c>
       <c r="D282" s="30">
-        <v>-121.6470267</v>
+        <v>-121.6595325</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5745,13 +5745,13 @@
         <v>391</v>
       </c>
       <c r="B283" s="30" t="s">
-        <v>329</v>
+        <v>394</v>
       </c>
       <c r="C283" s="30">
-        <v>38.279973130000002</v>
+        <v>38.263632440000002</v>
       </c>
       <c r="D283" s="30">
-        <v>-121.64155239999999</v>
+        <v>-121.6470267</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5759,13 +5759,13 @@
         <v>391</v>
       </c>
       <c r="B284" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C284" s="30">
-        <v>38.291833349999997</v>
+        <v>38.279973130000002</v>
       </c>
       <c r="D284" s="30">
-        <v>-121.6732488</v>
+        <v>-121.64155239999999</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5773,13 +5773,13 @@
         <v>391</v>
       </c>
       <c r="B285" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C285" s="30">
-        <v>38.192741210000001</v>
+        <v>38.291833349999997</v>
       </c>
       <c r="D285" s="30">
-        <v>-121.92653540000001</v>
+        <v>-121.6732488</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5787,13 +5787,13 @@
         <v>391</v>
       </c>
       <c r="B286" s="30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C286" s="30">
-        <v>38.293072469999998</v>
+        <v>38.192741210000001</v>
       </c>
       <c r="D286" s="30">
-        <v>-121.6861237</v>
+        <v>-121.92653540000001</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5801,13 +5801,13 @@
         <v>391</v>
       </c>
       <c r="B287" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C287" s="30">
-        <v>38.24394144</v>
+        <v>38.293072469999998</v>
       </c>
       <c r="D287" s="30">
-        <v>-121.66362479999999</v>
+        <v>-121.6861237</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5815,13 +5815,13 @@
         <v>391</v>
       </c>
       <c r="B288" s="30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C288" s="30">
-        <v>38.31306549</v>
+        <v>38.24394144</v>
       </c>
       <c r="D288" s="30">
-        <v>-121.66714140000001</v>
+        <v>-121.66362479999999</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5829,13 +5829,13 @@
         <v>391</v>
       </c>
       <c r="B289" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C289" s="30">
-        <v>38.081829999999997</v>
+        <v>38.31306549</v>
       </c>
       <c r="D289" s="30">
-        <v>-121.72399</v>
+        <v>-121.66714140000001</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5843,13 +5843,13 @@
         <v>391</v>
       </c>
       <c r="B290" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C290" s="30">
-        <v>38.083069999999999</v>
+        <v>38.081829999999997</v>
       </c>
       <c r="D290" s="30">
-        <v>-121.72206</v>
+        <v>-121.72399</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5857,13 +5857,13 @@
         <v>391</v>
       </c>
       <c r="B291" s="30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C291" s="30">
-        <v>38.08558</v>
+        <v>38.083069999999999</v>
       </c>
       <c r="D291" s="30">
-        <v>-121.70901000000001</v>
+        <v>-121.72206</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5871,13 +5871,13 @@
         <v>391</v>
       </c>
       <c r="B292" s="30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C292" s="30">
-        <v>38.08766</v>
+        <v>38.08558</v>
       </c>
       <c r="D292" s="30">
-        <v>-121.71127</v>
+        <v>-121.70901000000001</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -5885,13 +5885,13 @@
         <v>391</v>
       </c>
       <c r="B293" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C293" s="30">
-        <v>38.10013</v>
+        <v>38.08766</v>
       </c>
       <c r="D293" s="30">
-        <v>-121.70862</v>
+        <v>-121.71127</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -5899,13 +5899,13 @@
         <v>391</v>
       </c>
       <c r="B294" s="30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C294" s="30">
-        <v>38.100540000000002</v>
+        <v>38.10013</v>
       </c>
       <c r="D294" s="30">
-        <v>-121.70925</v>
+        <v>-121.70862</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -5913,13 +5913,13 @@
         <v>391</v>
       </c>
       <c r="B295" s="30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C295" s="30">
-        <v>38.080979999999997</v>
+        <v>38.100540000000002</v>
       </c>
       <c r="D295" s="30">
-        <v>-122.01718</v>
+        <v>-121.70925</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -5927,13 +5927,13 @@
         <v>391</v>
       </c>
       <c r="B296" s="30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C296" s="30">
-        <v>38.085477750000003</v>
+        <v>38.080979999999997</v>
       </c>
       <c r="D296" s="30">
-        <v>-122.01881400000001</v>
+        <v>-122.01718</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -5941,13 +5941,13 @@
         <v>391</v>
       </c>
       <c r="B297" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C297" s="30">
-        <v>38.083220560000001</v>
+        <v>38.085477750000003</v>
       </c>
       <c r="D297" s="30">
-        <v>-122.0083422</v>
+        <v>-122.01881400000001</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -5955,13 +5955,13 @@
         <v>391</v>
       </c>
       <c r="B298" s="30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C298" s="30">
-        <v>38.077246090000003</v>
+        <v>38.083220560000001</v>
       </c>
       <c r="D298" s="30">
-        <v>-122.0136547</v>
+        <v>-122.0083422</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -5969,13 +5969,13 @@
         <v>391</v>
       </c>
       <c r="B299" s="30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C299" s="30">
-        <v>38.077816849999998</v>
+        <v>38.077246090000003</v>
       </c>
       <c r="D299" s="30">
-        <v>-122.00347290000001</v>
+        <v>-122.0136547</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -5983,13 +5983,13 @@
         <v>391</v>
       </c>
       <c r="B300" s="30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C300" s="30">
-        <v>38.259108210000001</v>
+        <v>38.077816849999998</v>
       </c>
       <c r="D300" s="30">
-        <v>-121.677316</v>
+        <v>-122.00347290000001</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -5997,13 +5997,13 @@
         <v>391</v>
       </c>
       <c r="B301" s="30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C301" s="30">
-        <v>38.279969999999999</v>
+        <v>38.259108210000001</v>
       </c>
       <c r="D301" s="30">
-        <v>-121.69346</v>
+        <v>-121.677316</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -6011,13 +6011,13 @@
         <v>391</v>
       </c>
       <c r="B302" s="30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C302" s="30">
-        <v>38.309820799999997</v>
+        <v>38.279969999999999</v>
       </c>
       <c r="D302" s="30">
-        <v>-121.6928649</v>
+        <v>-121.69346</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6025,13 +6025,13 @@
         <v>391</v>
       </c>
       <c r="B303" s="30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C303" s="30">
-        <v>38.278499140000001</v>
+        <v>38.309820799999997</v>
       </c>
       <c r="D303" s="30">
-        <v>-121.6934933</v>
+        <v>-121.6928649</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -6039,13 +6039,13 @@
         <v>391</v>
       </c>
       <c r="B304" s="30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C304" s="30">
-        <v>38.032170000000001</v>
+        <v>38.278499140000001</v>
       </c>
       <c r="D304" s="30">
-        <v>-121.47817000000001</v>
+        <v>-121.6934933</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6053,13 +6053,13 @@
         <v>391</v>
       </c>
       <c r="B305" s="30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C305" s="30">
-        <v>38.03201</v>
+        <v>38.032170000000001</v>
       </c>
       <c r="D305" s="30">
-        <v>-121.47786000000001</v>
+        <v>-121.47817000000001</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6067,13 +6067,13 @@
         <v>391</v>
       </c>
       <c r="B306" s="30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C306" s="30">
-        <v>38.009160000000001</v>
+        <v>38.03201</v>
       </c>
       <c r="D306" s="30">
-        <v>-121.45679</v>
+        <v>-121.47786000000001</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6081,13 +6081,13 @@
         <v>391</v>
       </c>
       <c r="B307" s="30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C307" s="30">
-        <v>38.008040000000001</v>
+        <v>38.009160000000001</v>
       </c>
       <c r="D307" s="30">
-        <v>-121.45610000000001</v>
+        <v>-121.45679</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -6095,13 +6095,13 @@
         <v>391</v>
       </c>
       <c r="B308" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C308" s="30">
-        <v>38.003909999999998</v>
+        <v>38.008040000000001</v>
       </c>
       <c r="D308" s="30">
-        <v>-121.45036</v>
+        <v>-121.45610000000001</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -6109,13 +6109,13 @@
         <v>391</v>
       </c>
       <c r="B309" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C309" s="30">
-        <v>38.003450000000001</v>
+        <v>38.003909999999998</v>
       </c>
       <c r="D309" s="30">
-        <v>-121.45008</v>
+        <v>-121.45036</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -6123,13 +6123,13 @@
         <v>391</v>
       </c>
       <c r="B310" s="30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C310" s="30">
-        <v>37.997709999999998</v>
+        <v>38.003450000000001</v>
       </c>
       <c r="D310" s="30">
-        <v>-121.44746000000001</v>
+        <v>-121.45008</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6137,13 +6137,13 @@
         <v>391</v>
       </c>
       <c r="B311" s="30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C311" s="30">
-        <v>37.997520000000002</v>
+        <v>37.997709999999998</v>
       </c>
       <c r="D311" s="30">
-        <v>-121.44749</v>
+        <v>-121.44746000000001</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6151,13 +6151,13 @@
         <v>391</v>
       </c>
       <c r="B312" s="30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C312" s="30">
-        <v>38.249240190000002</v>
+        <v>37.997520000000002</v>
       </c>
       <c r="D312" s="30">
-        <v>-121.66372370000001</v>
+        <v>-121.44749</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6165,13 +6165,13 @@
         <v>391</v>
       </c>
       <c r="B313" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C313" s="30">
-        <v>38.244989259999997</v>
+        <v>38.249240190000002</v>
       </c>
       <c r="D313" s="30">
-        <v>-121.66946</v>
+        <v>-121.66372370000001</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6179,13 +6179,13 @@
         <v>391</v>
       </c>
       <c r="B314" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C314" s="30">
-        <v>38.238947359999997</v>
+        <v>38.244989259999997</v>
       </c>
       <c r="D314" s="30">
-        <v>-121.6687814</v>
+        <v>-121.66946</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6193,13 +6193,13 @@
         <v>391</v>
       </c>
       <c r="B315" s="30" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C315" s="30">
-        <v>38.251475419999998</v>
+        <v>38.238947359999997</v>
       </c>
       <c r="D315" s="30">
-        <v>-121.6603186</v>
+        <v>-121.6687814</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6207,13 +6207,13 @@
         <v>391</v>
       </c>
       <c r="B316" s="30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C316" s="30">
-        <v>38.24192</v>
+        <v>38.251475419999998</v>
       </c>
       <c r="D316" s="30">
-        <v>-121.66946</v>
+        <v>-121.6603186</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -6221,13 +6221,13 @@
         <v>391</v>
       </c>
       <c r="B317" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C317" s="30">
-        <v>38.237220000000001</v>
+        <v>38.24192</v>
       </c>
       <c r="D317" s="30">
-        <v>-121.6692</v>
+        <v>-121.66946</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -6235,13 +6235,13 @@
         <v>391</v>
       </c>
       <c r="B318" s="30" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C318" s="30">
-        <v>38.245260629999997</v>
+        <v>38.237220000000001</v>
       </c>
       <c r="D318" s="30">
-        <v>-121.6604141</v>
+        <v>-121.6692</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6249,37 +6249,37 @@
         <v>391</v>
       </c>
       <c r="B319" s="30" t="s">
-        <v>365</v>
-      </c>
-      <c r="C319" s="30"/>
-      <c r="D319" s="30"/>
+        <v>364</v>
+      </c>
+      <c r="C319" s="30">
+        <v>38.245260629999997</v>
+      </c>
+      <c r="D319" s="30">
+        <v>-121.6604141</v>
+      </c>
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B320" s="30" t="s">
-        <v>366</v>
-      </c>
-      <c r="C320" s="30">
-        <v>38.094700000000003</v>
-      </c>
-      <c r="D320" s="30">
-        <v>-121.59039</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="C320" s="30"/>
+      <c r="D320" s="30"/>
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="28" t="s">
         <v>391</v>
       </c>
       <c r="B321" s="30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C321" s="30">
-        <v>38.326660760000003</v>
+        <v>38.094700000000003</v>
       </c>
       <c r="D321" s="30">
-        <v>-121.68302919999999</v>
+        <v>-121.59039</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -6287,13 +6287,13 @@
         <v>391</v>
       </c>
       <c r="B322" s="30" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C322" s="30">
-        <v>38.333898980000001</v>
+        <v>38.326660760000003</v>
       </c>
       <c r="D322" s="30">
-        <v>-121.6739171</v>
+        <v>-121.68302919999999</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6301,13 +6301,13 @@
         <v>391</v>
       </c>
       <c r="B323" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C323" s="30">
-        <v>38.344457859999999</v>
+        <v>38.333898980000001</v>
       </c>
       <c r="D323" s="30">
-        <v>-121.6554718</v>
+        <v>-121.6739171</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -6315,13 +6315,13 @@
         <v>391</v>
       </c>
       <c r="B324" s="30" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C324" s="30">
-        <v>38.299759999999999</v>
+        <v>38.344457859999999</v>
       </c>
       <c r="D324" s="30">
-        <v>-121.68925</v>
+        <v>-121.6554718</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6329,13 +6329,13 @@
         <v>391</v>
       </c>
       <c r="B325" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C325" s="30">
-        <v>38.299639999999997</v>
+        <v>38.299759999999999</v>
       </c>
       <c r="D325" s="30">
-        <v>-121.69061000000001</v>
+        <v>-121.68925</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -6343,13 +6343,13 @@
         <v>391</v>
       </c>
       <c r="B326" s="30" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C326" s="30">
-        <v>38.261318639999999</v>
+        <v>38.299639999999997</v>
       </c>
       <c r="D326" s="30">
-        <v>-121.6860805</v>
+        <v>-121.69061000000001</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -6357,13 +6357,13 @@
         <v>391</v>
       </c>
       <c r="B327" s="30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C327" s="30">
-        <v>38.169350000000001</v>
+        <v>38.261318639999999</v>
       </c>
       <c r="D327" s="30">
-        <v>-121.41540999999999</v>
+        <v>-121.6860805</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -6371,13 +6371,13 @@
         <v>391</v>
       </c>
       <c r="B328" s="30" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C328" s="30">
-        <v>38.356349690000002</v>
+        <v>38.169350000000001</v>
       </c>
       <c r="D328" s="30">
-        <v>-121.6418877</v>
+        <v>-121.41540999999999</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6385,13 +6385,13 @@
         <v>391</v>
       </c>
       <c r="B329" s="30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C329" s="30">
-        <v>38.120756800000002</v>
+        <v>38.356349690000002</v>
       </c>
       <c r="D329" s="30">
-        <v>-121.9818389</v>
+        <v>-121.6418877</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -6399,13 +6399,13 @@
         <v>391</v>
       </c>
       <c r="B330" s="30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C330" s="30">
-        <v>38.122772070000003</v>
+        <v>38.120756800000002</v>
       </c>
       <c r="D330" s="30">
-        <v>-121.9860338</v>
+        <v>-121.9818389</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6413,13 +6413,13 @@
         <v>391</v>
       </c>
       <c r="B331" s="30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C331" s="30">
-        <v>38.128327800000001</v>
+        <v>38.122772070000003</v>
       </c>
       <c r="D331" s="30">
-        <v>-121.9895781</v>
+        <v>-121.9860338</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -6427,13 +6427,13 @@
         <v>391</v>
       </c>
       <c r="B332" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C332" s="30">
-        <v>38.134869999999999</v>
+        <v>38.128327800000001</v>
       </c>
       <c r="D332" s="30">
-        <v>-121.99668</v>
+        <v>-121.9895781</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -6441,7 +6441,7 @@
         <v>391</v>
       </c>
       <c r="B333" s="30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C333" s="30">
         <v>38.134869999999999</v>
@@ -6455,13 +6455,13 @@
         <v>391</v>
       </c>
       <c r="B334" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C334" s="30">
-        <v>38.113599999999998</v>
+        <v>38.134869999999999</v>
       </c>
       <c r="D334" s="30">
-        <v>-121.98169</v>
+        <v>-121.99668</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6469,13 +6469,13 @@
         <v>391</v>
       </c>
       <c r="B335" s="30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C335" s="30">
-        <v>38.113779999999998</v>
+        <v>38.113599999999998</v>
       </c>
       <c r="D335" s="30">
-        <v>-121.98161</v>
+        <v>-121.98169</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -6483,13 +6483,13 @@
         <v>391</v>
       </c>
       <c r="B336" s="30" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C336" s="30">
-        <v>38.09502792</v>
+        <v>38.113779999999998</v>
       </c>
       <c r="D336" s="30">
-        <v>-121.5879041</v>
+        <v>-121.98161</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -6497,13 +6497,13 @@
         <v>391</v>
       </c>
       <c r="B337" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C337" s="30">
-        <v>38.334020000000002</v>
+        <v>38.09502792</v>
       </c>
       <c r="D337" s="30">
-        <v>-121.67107</v>
+        <v>-121.5879041</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -6511,13 +6511,13 @@
         <v>391</v>
       </c>
       <c r="B338" s="30" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="C338" s="30">
-        <v>38.045928529999998</v>
+        <v>38.334020000000002</v>
       </c>
       <c r="D338" s="30">
-        <v>-121.84750099999999</v>
+        <v>-121.67107</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -6525,13 +6525,13 @@
         <v>391</v>
       </c>
       <c r="B339" s="30" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="C339" s="30">
-        <v>38.226939999999999</v>
+        <v>38.045928529999998</v>
       </c>
       <c r="D339" s="30">
-        <v>-122.03591</v>
+        <v>-121.84750099999999</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -6539,13 +6539,13 @@
         <v>391</v>
       </c>
       <c r="B340" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C340" s="30">
-        <v>38.226010000000002</v>
+        <v>38.226939999999999</v>
       </c>
       <c r="D340" s="30">
-        <v>-122.03825999999999</v>
+        <v>-122.03591</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -6553,13 +6553,13 @@
         <v>391</v>
       </c>
       <c r="B341" s="30" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C341" s="30">
-        <v>38.049653829999997</v>
+        <v>38.226010000000002</v>
       </c>
       <c r="D341" s="30">
-        <v>-121.8488996</v>
+        <v>-122.03825999999999</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6567,13 +6567,13 @@
         <v>391</v>
       </c>
       <c r="B342" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C342" s="30">
-        <v>38.037943380000002</v>
+        <v>38.049653829999997</v>
       </c>
       <c r="D342" s="30">
-        <v>-121.84428459999999</v>
+        <v>-121.8488996</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -6581,13 +6581,13 @@
         <v>391</v>
       </c>
       <c r="B343" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C343" s="30">
-        <v>38.030609779999999</v>
+        <v>38.037943380000002</v>
       </c>
       <c r="D343" s="30">
-        <v>-121.8414193</v>
+        <v>-121.84428459999999</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -6595,13 +6595,13 @@
         <v>391</v>
       </c>
       <c r="B344" s="30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C344" s="30">
-        <v>38.052289080000001</v>
+        <v>38.030609779999999</v>
       </c>
       <c r="D344" s="30">
-        <v>-121.85680499999999</v>
+        <v>-121.8414193</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -6609,27 +6609,27 @@
         <v>391</v>
       </c>
       <c r="B345" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="C345" s="30">
+        <v>38.052289080000001</v>
+      </c>
+      <c r="D345" s="30">
+        <v>-121.85680499999999</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4">
+      <c r="A346" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="B346" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="C345" s="30">
+      <c r="C346" s="30">
         <v>38.052123680000001</v>
       </c>
-      <c r="D345" s="30">
+      <c r="D346" s="30">
         <v>-121.8542861</v>
-      </c>
-    </row>
-    <row r="346" spans="1:4">
-      <c r="A346" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="B346">
-        <v>340</v>
-      </c>
-      <c r="C346">
-        <v>38.105080000000001</v>
-      </c>
-      <c r="D346">
-        <v>-122.26988</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -6637,13 +6637,13 @@
         <v>198</v>
       </c>
       <c r="B347">
-        <v>405</v>
+        <v>340</v>
       </c>
       <c r="C347">
-        <v>38.033529999999999</v>
+        <v>38.105080000000001</v>
       </c>
       <c r="D347">
-        <v>-122.15815000000001</v>
+        <v>-122.26988</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6651,13 +6651,13 @@
         <v>198</v>
       </c>
       <c r="B348">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C348">
-        <v>38.061169999999997</v>
+        <v>38.033529999999999</v>
       </c>
       <c r="D348">
-        <v>-122.06828</v>
+        <v>-122.15815000000001</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6665,13 +6665,13 @@
         <v>198</v>
       </c>
       <c r="B349">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C349">
-        <v>38.0702</v>
+        <v>38.061169999999997</v>
       </c>
       <c r="D349">
-        <v>-122.09415</v>
+        <v>-122.06828</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6679,13 +6679,13 @@
         <v>198</v>
       </c>
       <c r="B350">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C350">
-        <v>38.093829999999997</v>
+        <v>38.0702</v>
       </c>
       <c r="D350">
-        <v>-122.06973000000001</v>
+        <v>-122.09415</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6693,13 +6693,13 @@
         <v>198</v>
       </c>
       <c r="B351">
-        <v>501</v>
+        <v>418</v>
       </c>
       <c r="C351">
-        <v>38.061669999999999</v>
+        <v>38.093829999999997</v>
       </c>
       <c r="D351">
-        <v>-122.01955</v>
+        <v>-122.06973000000001</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6707,13 +6707,13 @@
         <v>198</v>
       </c>
       <c r="B352">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C352">
-        <v>38.05997</v>
+        <v>38.061669999999999</v>
       </c>
       <c r="D352">
-        <v>-122.00397</v>
+        <v>-122.01955</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -6721,13 +6721,13 @@
         <v>198</v>
       </c>
       <c r="B353">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C353">
-        <v>38.059449999999998</v>
+        <v>38.05997</v>
       </c>
       <c r="D353">
-        <v>-121.97669999999999</v>
+        <v>-122.00397</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6735,13 +6735,13 @@
         <v>198</v>
       </c>
       <c r="B354">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C354">
-        <v>38.04813</v>
+        <v>38.059449999999998</v>
       </c>
       <c r="D354">
-        <v>-121.91492</v>
+        <v>-121.97669999999999</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6749,13 +6749,13 @@
         <v>198</v>
       </c>
       <c r="B355">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="C355">
-        <v>38.059199999999997</v>
+        <v>38.04813</v>
       </c>
       <c r="D355">
-        <v>-121.86842</v>
+        <v>-121.91492</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -6763,13 +6763,13 @@
         <v>198</v>
       </c>
       <c r="B356">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C356">
-        <v>38.073779999999999</v>
+        <v>38.059199999999997</v>
       </c>
       <c r="D356">
-        <v>-121.94725</v>
+        <v>-121.86842</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6777,13 +6777,13 @@
         <v>198</v>
       </c>
       <c r="B357">
-        <v>602</v>
+        <v>519</v>
       </c>
       <c r="C357">
-        <v>38.117829999999998</v>
+        <v>38.073779999999999</v>
       </c>
       <c r="D357">
-        <v>-122.04183</v>
+        <v>-121.94725</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6791,13 +6791,13 @@
         <v>198</v>
       </c>
       <c r="B358">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C358">
-        <v>38.148530000000001</v>
+        <v>38.117829999999998</v>
       </c>
       <c r="D358">
-        <v>-122.05737999999999</v>
+        <v>-122.04183</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6805,13 +6805,13 @@
         <v>198</v>
       </c>
       <c r="B359">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C359">
-        <v>38.169800000000002</v>
+        <v>38.148530000000001</v>
       </c>
       <c r="D359">
-        <v>-122.02177</v>
+        <v>-122.05737999999999</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6819,13 +6819,13 @@
         <v>198</v>
       </c>
       <c r="B360">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C360">
-        <v>38.088700000000003</v>
+        <v>38.169800000000002</v>
       </c>
       <c r="D360">
-        <v>-121.88332</v>
+        <v>-122.02177</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6833,13 +6833,13 @@
         <v>198</v>
       </c>
       <c r="B361">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C361">
-        <v>38.16771</v>
+        <v>38.088700000000003</v>
       </c>
       <c r="D361">
-        <v>-121.93470000000001</v>
+        <v>-121.88332</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6847,13 +6847,13 @@
         <v>198</v>
       </c>
       <c r="B362">
-        <v>704</v>
+        <v>609</v>
       </c>
       <c r="C362">
-        <v>38.070869999999999</v>
+        <v>38.16771</v>
       </c>
       <c r="D362">
-        <v>-121.77892</v>
+        <v>-121.93470000000001</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6861,13 +6861,13 @@
         <v>198</v>
       </c>
       <c r="B363">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C363">
-        <v>38.090299999999999</v>
+        <v>38.070869999999999</v>
       </c>
       <c r="D363">
-        <v>-121.74</v>
+        <v>-121.77892</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -6875,13 +6875,13 @@
         <v>198</v>
       </c>
       <c r="B364">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C364">
-        <v>38.113970000000002</v>
+        <v>38.090299999999999</v>
       </c>
       <c r="D364">
-        <v>-121.70797</v>
+        <v>-121.74</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -6889,13 +6889,13 @@
         <v>198</v>
       </c>
       <c r="B365">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C365">
-        <v>38.17595</v>
+        <v>38.113970000000002</v>
       </c>
       <c r="D365">
-        <v>-121.67028000000001</v>
+        <v>-121.70797</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -6903,13 +6903,13 @@
         <v>198</v>
       </c>
       <c r="B366">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="C366">
-        <v>38.237870000000001</v>
+        <v>38.17595</v>
       </c>
       <c r="D366">
-        <v>-121.68438</v>
+        <v>-121.67028000000001</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -6917,13 +6917,13 @@
         <v>198</v>
       </c>
       <c r="B367">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C367">
-        <v>38.33428</v>
+        <v>38.237870000000001</v>
       </c>
       <c r="D367">
-        <v>-121.64733</v>
+        <v>-121.68438</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -6931,13 +6931,13 @@
         <v>198</v>
       </c>
       <c r="B368">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C368">
-        <v>38.268149999999999</v>
+        <v>38.33428</v>
       </c>
       <c r="D368">
-        <v>-121.70277</v>
+        <v>-121.64733</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -6945,13 +6945,13 @@
         <v>198</v>
       </c>
       <c r="B369">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C369">
-        <v>38.236150000000002</v>
+        <v>38.268149999999999</v>
       </c>
       <c r="D369">
-        <v>-121.67348</v>
+        <v>-121.70277</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -6959,13 +6959,13 @@
         <v>198</v>
       </c>
       <c r="B370">
-        <v>795</v>
+        <v>723</v>
       </c>
       <c r="C370">
-        <v>38.537700000000001</v>
+        <v>38.236150000000002</v>
       </c>
       <c r="D370">
-        <v>-121.58468000000001</v>
+        <v>-121.67348</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -6973,13 +6973,13 @@
         <v>198</v>
       </c>
       <c r="B371">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C371">
-        <v>38.473869999999998</v>
+        <v>38.537700000000001</v>
       </c>
       <c r="D371">
-        <v>-121.5844</v>
+        <v>-121.58468000000001</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -6987,13 +6987,13 @@
         <v>198</v>
       </c>
       <c r="B372">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C372">
-        <v>38.404620000000001</v>
+        <v>38.473869999999998</v>
       </c>
       <c r="D372">
-        <v>-121.6156</v>
+        <v>-121.5844</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -7001,13 +7001,13 @@
         <v>198</v>
       </c>
       <c r="B373">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="C373">
-        <v>38.03528</v>
+        <v>38.404620000000001</v>
       </c>
       <c r="D373">
-        <v>-121.83875</v>
+        <v>-121.6156</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7015,13 +7015,13 @@
         <v>198</v>
       </c>
       <c r="B374">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C374">
-        <v>38.02308</v>
+        <v>38.03528</v>
       </c>
       <c r="D374">
-        <v>-121.79868</v>
+        <v>-121.83875</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7029,13 +7029,13 @@
         <v>198</v>
       </c>
       <c r="B375">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="C375">
-        <v>38.051200000000001</v>
+        <v>38.02308</v>
       </c>
       <c r="D375">
-        <v>-121.69305</v>
+        <v>-121.79868</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7043,13 +7043,13 @@
         <v>198</v>
       </c>
       <c r="B376">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="C376">
-        <v>38.087919999999997</v>
+        <v>38.051200000000001</v>
       </c>
       <c r="D376">
-        <v>-121.64883</v>
+        <v>-121.69305</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7057,13 +7057,13 @@
         <v>198</v>
       </c>
       <c r="B377">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C377">
-        <v>38.091299999999997</v>
+        <v>38.087919999999997</v>
       </c>
       <c r="D377">
-        <v>-121.57586999999999</v>
+        <v>-121.64883</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7071,13 +7071,13 @@
         <v>198</v>
       </c>
       <c r="B378">
-        <v>902</v>
+        <v>815</v>
       </c>
       <c r="C378">
-        <v>38.020499999999998</v>
+        <v>38.091299999999997</v>
       </c>
       <c r="D378">
-        <v>-121.58255</v>
+        <v>-121.57586999999999</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7085,13 +7085,13 @@
         <v>198</v>
       </c>
       <c r="B379">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C379">
-        <v>38.054119999999998</v>
+        <v>38.020499999999998</v>
       </c>
       <c r="D379">
-        <v>-121.51653</v>
+        <v>-121.58255</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7099,13 +7099,13 @@
         <v>198</v>
       </c>
       <c r="B380">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C380">
-        <v>38.002279999999999</v>
+        <v>38.054119999999998</v>
       </c>
       <c r="D380">
-        <v>-121.45037000000001</v>
+        <v>-121.51653</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7113,13 +7113,13 @@
         <v>198</v>
       </c>
       <c r="B381">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C381">
-        <v>37.968829999999997</v>
+        <v>38.002279999999999</v>
       </c>
       <c r="D381">
-        <v>-121.37172</v>
+        <v>-121.45037000000001</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7127,13 +7127,13 @@
         <v>198</v>
       </c>
       <c r="B382">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C382">
-        <v>37.946620000000003</v>
+        <v>37.968829999999997</v>
       </c>
       <c r="D382">
-        <v>-121.53475</v>
+        <v>-121.37172</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7141,13 +7141,13 @@
         <v>198</v>
       </c>
       <c r="B383">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C383">
-        <v>37.948999999999998</v>
+        <v>37.946620000000003</v>
       </c>
       <c r="D383">
-        <v>-121.55907999999999</v>
+        <v>-121.53475</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7155,41 +7155,41 @@
         <v>198</v>
       </c>
       <c r="B384">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="C384">
-        <v>38.105719999999998</v>
+        <v>37.948999999999998</v>
       </c>
       <c r="D384">
-        <v>-121.49525</v>
+        <v>-121.55907999999999</v>
       </c>
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="B385" s="28" t="s">
+      <c r="B385">
+        <v>919</v>
+      </c>
+      <c r="C385">
+        <v>38.105719999999998</v>
+      </c>
+      <c r="D385">
+        <v>-121.49525</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4">
+      <c r="A386" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B386" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="C385" s="29">
+      <c r="C386" s="29">
         <v>38.0328055556</v>
       </c>
-      <c r="D385" s="29">
+      <c r="D386" s="29">
         <v>-121.869305556</v>
-      </c>
-    </row>
-    <row r="386" spans="1:4">
-      <c r="A386" s="28" t="s">
-        <v>402</v>
-      </c>
-      <c r="B386" t="s">
-        <v>403</v>
-      </c>
-      <c r="C386">
-        <v>38.531880999999998</v>
-      </c>
-      <c r="D386">
-        <v>-121.527912</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -7197,19 +7197,28 @@
         <v>402</v>
       </c>
       <c r="B387" t="s">
+        <v>403</v>
+      </c>
+      <c r="C387">
+        <v>38.531880999999998</v>
+      </c>
+      <c r="D387">
+        <v>-121.527912</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4">
+      <c r="A388" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B388" t="s">
         <v>404</v>
       </c>
-      <c r="C387">
+      <c r="C388">
         <v>38.353383000000001</v>
       </c>
-      <c r="D387">
+      <c r="D388">
         <v>-121.643181</v>
       </c>
-    </row>
-    <row r="388" spans="1:4">
-      <c r="B388" s="34"/>
-      <c r="C388" s="36"/>
-      <c r="D388" s="36"/>
     </row>
     <row r="389" spans="1:4">
       <c r="B389" s="34"/>
@@ -7218,13 +7227,13 @@
     </row>
     <row r="390" spans="1:4">
       <c r="B390" s="34"/>
-      <c r="C390" s="37"/>
-      <c r="D390" s="35"/>
+      <c r="C390" s="36"/>
+      <c r="D390" s="36"/>
     </row>
     <row r="391" spans="1:4">
       <c r="B391" s="34"/>
       <c r="C391" s="37"/>
-      <c r="D391" s="38"/>
+      <c r="D391" s="35"/>
     </row>
     <row r="392" spans="1:4">
       <c r="B392" s="34"/>
@@ -7235,6 +7244,11 @@
       <c r="B393" s="34"/>
       <c r="C393" s="37"/>
       <c r="D393" s="38"/>
+    </row>
+    <row r="394" spans="1:4">
+      <c r="B394" s="34"/>
+      <c r="C394" s="37"/>
+      <c r="D394" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>